<commit_message>
Actualización de formulas en la pestaña de "estimacion de Esfuerzo"
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/2. Estimación y Planeación/Plantillas estimación/PTLL_Estimación_Esfuerzo.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/2. Estimación y Planeación/Plantillas estimación/PTLL_Estimación_Esfuerzo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="-105" windowWidth="8490" windowHeight="7425" tabRatio="710" activeTab="1"/>
+    <workbookView xWindow="6810" yWindow="-105" windowWidth="8490" windowHeight="7425" tabRatio="710" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="36" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="193">
   <si>
     <t>Nº</t>
   </si>
@@ -490,9 +490,6 @@
   </si>
   <si>
     <t>Ejecución de los casos de prueba</t>
-  </si>
-  <si>
-    <t>Verificación y corrección de los defectos</t>
   </si>
   <si>
     <t>Costo Total del desarrollo del  Proyecto</t>
@@ -715,9 +712,6 @@
     <t>Definir el plan de pruebas</t>
   </si>
   <si>
-    <t>Aprobación del polan de proyecto</t>
-  </si>
-  <si>
     <t>Definir la arquitectura del proyecto</t>
   </si>
   <si>
@@ -758,6 +752,15 @@
       </rPr>
       <t>: Se refiere a la dificultas que el Factor de Complejidad ya sea Técnico o Ambiental puede presentar cuando se realice el proyecto. Los valores dentro de complejidad son fijos y no estan sujetos a cambios.</t>
     </r>
+  </si>
+  <si>
+    <t>Corrección de los defectos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificación </t>
+  </si>
+  <si>
+    <t>Aprobación del plan de proyecto</t>
   </si>
 </sst>
 </file>
@@ -1579,12 +1582,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="250">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1713,9 +1717,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="25" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="25" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1844,9 +1845,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1966,54 +1964,6 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2042,200 +1992,268 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje 2" xfId="3"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -3073,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IV43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3085,28 +3103,28 @@
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="170" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="169"/>
-      <c r="B2" s="177" t="s">
+    <row r="2" spans="1:7" s="168" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="167"/>
+      <c r="B2" s="212" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="212"/>
+      <c r="D2" s="213" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="178" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-    </row>
-    <row r="4" spans="1:7" s="168" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="167"/>
-      <c r="B4" s="171" t="s">
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+    </row>
+    <row r="4" spans="1:7" s="166" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="165"/>
+      <c r="B4" s="169" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
+      <c r="F4" s="165"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -3145,19 +3163,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="168" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="167"/>
-      <c r="B12" s="171" t="s">
+    <row r="12" spans="1:7" s="166" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="165"/>
+      <c r="B12" s="169" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="167"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="167"/>
-      <c r="F12" s="167"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="165"/>
+      <c r="F12" s="165"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3287,20 +3305,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:256" s="168" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A31" s="167"/>
-      <c r="B31" s="171" t="s">
+    <row r="31" spans="1:256" s="166" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="165"/>
+      <c r="B31" s="169" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
+      <c r="C31" s="165"/>
+      <c r="D31" s="165"/>
+      <c r="E31" s="165"/>
+      <c r="F31" s="165"/>
     </row>
     <row r="32" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -3910,640 +3928,652 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="200" customWidth="1"/>
-    <col min="2" max="2" width="15" style="200" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="200" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="200" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="200" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="200" customWidth="1"/>
-    <col min="7" max="7" width="46.140625" style="200" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="200" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="200"/>
+    <col min="1" max="1" width="5.28515625" style="182" customWidth="1"/>
+    <col min="2" max="2" width="15" style="182" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" style="182" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="182" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="182" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="182" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" style="182" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="182" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="182"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="181" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="201" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="201"/>
-      <c r="G3" s="201"/>
-      <c r="H3" s="201"/>
+      <c r="B3" s="232" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="232"/>
+      <c r="D3" s="232"/>
+      <c r="E3" s="232"/>
+      <c r="F3" s="232"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="232"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="247" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="247"/>
-      <c r="D4" s="247"/>
-      <c r="E4" s="247"/>
-      <c r="F4" s="247"/>
-      <c r="G4" s="247"/>
-      <c r="H4" s="247"/>
+      <c r="B4" s="233" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
+      <c r="E4" s="233"/>
+      <c r="F4" s="233"/>
+      <c r="G4" s="233"/>
+      <c r="H4" s="233"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="247"/>
-      <c r="C5" s="247"/>
-      <c r="D5" s="247"/>
-      <c r="E5" s="247"/>
-      <c r="F5" s="247"/>
-      <c r="G5" s="247"/>
-      <c r="H5" s="247"/>
+      <c r="B5" s="233"/>
+      <c r="C5" s="233"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="233"/>
+      <c r="H5" s="233"/>
     </row>
     <row r="8" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="202" t="s">
+      <c r="B8" s="227" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="203"/>
-      <c r="D8" s="203"/>
-      <c r="E8" s="203"/>
-      <c r="F8" s="203"/>
-      <c r="G8" s="203"/>
-      <c r="H8" s="204"/>
+      <c r="C8" s="228"/>
+      <c r="D8" s="228"/>
+      <c r="E8" s="228"/>
+      <c r="F8" s="228"/>
+      <c r="G8" s="228"/>
+      <c r="H8" s="229"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="205"/>
-      <c r="C9" s="206"/>
-      <c r="D9" s="206"/>
-      <c r="E9" s="206"/>
-      <c r="F9" s="206"/>
-      <c r="G9" s="206" t="s">
+      <c r="B9" s="183"/>
+      <c r="C9" s="184"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="184" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="207">
+      <c r="H9" s="185">
         <f>0.6+(0.01*SUM(F11:F23))</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="208" t="s">
+      <c r="B10" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="209" t="s">
+      <c r="C10" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="210" t="s">
+      <c r="D10" s="188" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="210" t="s">
+      <c r="E10" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="208" t="s">
+      <c r="F10" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="211" t="s">
+      <c r="G10" s="230" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="212"/>
+      <c r="H10" s="231"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="189" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="214" t="s">
+      <c r="C11" s="190" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="193">
+      <c r="D11" s="175">
         <v>2</v>
       </c>
-      <c r="E11" s="215">
-        <v>0</v>
-      </c>
-      <c r="F11" s="196">
+      <c r="E11" s="191">
+        <v>0</v>
+      </c>
+      <c r="F11" s="178">
         <f t="shared" ref="F11:F23" si="0">E11*D11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="216"/>
-      <c r="H11" s="217"/>
-      <c r="K11" s="218"/>
+      <c r="G11" s="225"/>
+      <c r="H11" s="226"/>
+      <c r="K11" s="192"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="219" t="s">
+      <c r="B12" s="193" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="218" t="s">
+      <c r="C12" s="192" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="194">
+      <c r="D12" s="176">
         <v>2</v>
       </c>
-      <c r="E12" s="220">
-        <v>0</v>
-      </c>
-      <c r="F12" s="197">
+      <c r="E12" s="194">
+        <v>0</v>
+      </c>
+      <c r="F12" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="221"/>
-      <c r="H12" s="222"/>
+      <c r="G12" s="216"/>
+      <c r="H12" s="217"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="219" t="s">
+      <c r="B13" s="193" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="218" t="s">
+      <c r="C13" s="192" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="194">
+      <c r="D13" s="176">
         <v>1</v>
       </c>
-      <c r="E13" s="220">
-        <v>0</v>
-      </c>
-      <c r="F13" s="197">
+      <c r="E13" s="194">
+        <v>0</v>
+      </c>
+      <c r="F13" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="221"/>
-      <c r="H13" s="222"/>
+      <c r="G13" s="216"/>
+      <c r="H13" s="217"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="219" t="s">
+      <c r="B14" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="218" t="s">
+      <c r="C14" s="192" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="194">
+      <c r="D14" s="176">
         <v>1</v>
       </c>
-      <c r="E14" s="220">
-        <v>0</v>
-      </c>
-      <c r="F14" s="197">
+      <c r="E14" s="194">
+        <v>0</v>
+      </c>
+      <c r="F14" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="221"/>
-      <c r="H14" s="222"/>
+      <c r="G14" s="216"/>
+      <c r="H14" s="217"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="219" t="s">
+      <c r="B15" s="193" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="218" t="s">
+      <c r="C15" s="192" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="194">
+      <c r="D15" s="176">
         <v>1</v>
       </c>
-      <c r="E15" s="220">
-        <v>0</v>
-      </c>
-      <c r="F15" s="197">
+      <c r="E15" s="194">
+        <v>0</v>
+      </c>
+      <c r="F15" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="221"/>
-      <c r="H15" s="222"/>
+      <c r="G15" s="216"/>
+      <c r="H15" s="217"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="219" t="s">
+      <c r="B16" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="218" t="s">
+      <c r="C16" s="192" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="194">
+      <c r="D16" s="176">
         <v>0.5</v>
       </c>
-      <c r="E16" s="220">
-        <v>0</v>
-      </c>
-      <c r="F16" s="197">
+      <c r="E16" s="194">
+        <v>0</v>
+      </c>
+      <c r="F16" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="218"/>
-      <c r="H16" s="223"/>
+      <c r="G16" s="192"/>
+      <c r="H16" s="195"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="219" t="s">
+      <c r="B17" s="193" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="218" t="s">
+      <c r="C17" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="194">
+      <c r="D17" s="176">
         <v>0.5</v>
       </c>
-      <c r="E17" s="220">
-        <v>0</v>
-      </c>
-      <c r="F17" s="197">
+      <c r="E17" s="194">
+        <v>0</v>
+      </c>
+      <c r="F17" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="221"/>
-      <c r="H17" s="222"/>
+      <c r="G17" s="216"/>
+      <c r="H17" s="217"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="219" t="s">
+      <c r="B18" s="193" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="218" t="s">
+      <c r="C18" s="192" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="194">
+      <c r="D18" s="176">
         <v>2</v>
       </c>
-      <c r="E18" s="220">
-        <v>0</v>
-      </c>
-      <c r="F18" s="197">
+      <c r="E18" s="194">
+        <v>0</v>
+      </c>
+      <c r="F18" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="218"/>
-      <c r="H18" s="223"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="195"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="219" t="s">
+      <c r="B19" s="193" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="218" t="s">
+      <c r="C19" s="192" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="194">
+      <c r="D19" s="176">
         <v>1</v>
       </c>
-      <c r="E19" s="220">
-        <v>0</v>
-      </c>
-      <c r="F19" s="197">
+      <c r="E19" s="194">
+        <v>0</v>
+      </c>
+      <c r="F19" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="221"/>
-      <c r="H19" s="222"/>
+      <c r="G19" s="216"/>
+      <c r="H19" s="217"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="219" t="s">
+      <c r="B20" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="218" t="s">
+      <c r="C20" s="192" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="194">
+      <c r="D20" s="176">
         <v>1</v>
       </c>
-      <c r="E20" s="220">
-        <v>0</v>
-      </c>
-      <c r="F20" s="197">
+      <c r="E20" s="194">
+        <v>0</v>
+      </c>
+      <c r="F20" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="221"/>
-      <c r="H20" s="222"/>
+      <c r="G20" s="216"/>
+      <c r="H20" s="217"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="193" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="218" t="s">
+      <c r="C21" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="194">
+      <c r="D21" s="176">
         <v>1</v>
       </c>
-      <c r="E21" s="220">
-        <v>0</v>
-      </c>
-      <c r="F21" s="197">
+      <c r="E21" s="194">
+        <v>0</v>
+      </c>
+      <c r="F21" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="221"/>
-      <c r="H21" s="222"/>
+      <c r="G21" s="216"/>
+      <c r="H21" s="217"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="219" t="s">
+      <c r="B22" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="218" t="s">
+      <c r="C22" s="192" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="194">
+      <c r="D22" s="176">
         <v>1</v>
       </c>
-      <c r="E22" s="220">
-        <v>0</v>
-      </c>
-      <c r="F22" s="197">
+      <c r="E22" s="194">
+        <v>0</v>
+      </c>
+      <c r="F22" s="179">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="221"/>
-      <c r="H22" s="222"/>
+      <c r="G22" s="216"/>
+      <c r="H22" s="217"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="224" t="s">
+      <c r="B23" s="196" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="225" t="s">
+      <c r="C23" s="197" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="195">
+      <c r="D23" s="177">
         <v>1</v>
       </c>
-      <c r="E23" s="226">
-        <v>0</v>
-      </c>
-      <c r="F23" s="198">
+      <c r="E23" s="198">
+        <v>0</v>
+      </c>
+      <c r="F23" s="180">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="221"/>
-      <c r="H23" s="222"/>
+      <c r="G23" s="216"/>
+      <c r="H23" s="217"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="227"/>
-      <c r="C24" s="228"/>
-      <c r="D24" s="228"/>
-      <c r="E24" s="228" t="s">
+      <c r="B24" s="199"/>
+      <c r="C24" s="200"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="200" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="229">
+      <c r="F24" s="201">
         <f>SUM(F11:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="228"/>
-      <c r="H24" s="230"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="202"/>
     </row>
     <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="202" t="s">
+      <c r="B27" s="227" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="203"/>
-      <c r="D27" s="203"/>
-      <c r="E27" s="203"/>
-      <c r="F27" s="203"/>
-      <c r="G27" s="203"/>
-      <c r="H27" s="204"/>
+      <c r="C27" s="228"/>
+      <c r="D27" s="228"/>
+      <c r="E27" s="228"/>
+      <c r="F27" s="228"/>
+      <c r="G27" s="228"/>
+      <c r="H27" s="229"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B28" s="206"/>
-      <c r="C28" s="206"/>
-      <c r="D28" s="206"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206" t="s">
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="184" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="206">
+      <c r="H28" s="184">
         <f>1.4+(-0.03*SUM(F30:F37))</f>
         <v>1.4</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="208" t="s">
+      <c r="B29" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="209" t="s">
+      <c r="C29" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="210" t="s">
+      <c r="D29" s="188" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="210" t="s">
+      <c r="E29" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="208" t="s">
+      <c r="F29" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="211" t="s">
+      <c r="G29" s="230" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="212"/>
+      <c r="H29" s="231"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="213" t="s">
+      <c r="B30" s="189" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="231" t="s">
+      <c r="C30" s="203" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="248">
+      <c r="D30" s="210">
         <v>1.5</v>
       </c>
-      <c r="E30" s="215">
-        <v>0</v>
-      </c>
-      <c r="F30" s="232">
+      <c r="E30" s="191">
+        <v>0</v>
+      </c>
+      <c r="F30" s="204">
         <f t="shared" ref="F30:F37" si="1">E30*D30</f>
         <v>0</v>
       </c>
-      <c r="G30" s="216"/>
-      <c r="H30" s="217"/>
+      <c r="G30" s="225"/>
+      <c r="H30" s="226"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="219" t="s">
+      <c r="B31" s="193" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="218" t="s">
+      <c r="C31" s="192" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="249">
+      <c r="D31" s="211">
         <v>0.5</v>
       </c>
-      <c r="E31" s="220">
-        <v>0</v>
-      </c>
-      <c r="F31" s="233">
+      <c r="E31" s="194">
+        <v>0</v>
+      </c>
+      <c r="F31" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G31" s="221"/>
-      <c r="H31" s="222"/>
+      <c r="G31" s="216"/>
+      <c r="H31" s="217"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="219" t="s">
+      <c r="B32" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="218" t="s">
+      <c r="C32" s="192" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="249">
+      <c r="D32" s="211">
         <v>1</v>
       </c>
-      <c r="E32" s="220">
-        <v>0</v>
-      </c>
-      <c r="F32" s="233">
+      <c r="E32" s="194">
+        <v>0</v>
+      </c>
+      <c r="F32" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="221"/>
-      <c r="H32" s="222"/>
+      <c r="G32" s="216"/>
+      <c r="H32" s="217"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="219" t="s">
+      <c r="B33" s="193" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="218" t="s">
+      <c r="C33" s="192" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="249">
+      <c r="D33" s="211">
         <v>0.5</v>
       </c>
-      <c r="E33" s="220">
-        <v>0</v>
-      </c>
-      <c r="F33" s="233">
+      <c r="E33" s="194">
+        <v>0</v>
+      </c>
+      <c r="F33" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G33" s="221"/>
-      <c r="H33" s="222"/>
+      <c r="G33" s="216"/>
+      <c r="H33" s="217"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="219" t="s">
+      <c r="B34" s="193" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="218" t="s">
+      <c r="C34" s="192" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="249">
+      <c r="D34" s="211">
         <v>1</v>
       </c>
-      <c r="E34" s="220">
-        <v>0</v>
-      </c>
-      <c r="F34" s="233">
+      <c r="E34" s="194">
+        <v>0</v>
+      </c>
+      <c r="F34" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G34" s="221"/>
-      <c r="H34" s="222"/>
+      <c r="G34" s="216"/>
+      <c r="H34" s="217"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="219" t="s">
+      <c r="B35" s="193" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="218" t="s">
+      <c r="C35" s="192" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="249">
+      <c r="D35" s="211">
         <v>2</v>
       </c>
-      <c r="E35" s="220">
-        <v>0</v>
-      </c>
-      <c r="F35" s="233">
+      <c r="E35" s="194">
+        <v>0</v>
+      </c>
+      <c r="F35" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G35" s="218"/>
-      <c r="H35" s="223"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="195"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="219" t="s">
+      <c r="B36" s="193" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="218" t="s">
+      <c r="C36" s="192" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="249">
+      <c r="D36" s="211">
         <v>-1</v>
       </c>
-      <c r="E36" s="220">
-        <v>0</v>
-      </c>
-      <c r="F36" s="233">
+      <c r="E36" s="194">
+        <v>0</v>
+      </c>
+      <c r="F36" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36" s="221"/>
-      <c r="H36" s="222"/>
+      <c r="G36" s="216"/>
+      <c r="H36" s="217"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="219" t="s">
+      <c r="B37" s="193" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="218" t="s">
+      <c r="C37" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="249">
+      <c r="D37" s="211">
         <v>2</v>
       </c>
-      <c r="E37" s="220">
-        <v>0</v>
-      </c>
-      <c r="F37" s="233">
+      <c r="E37" s="194">
+        <v>0</v>
+      </c>
+      <c r="F37" s="205">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G37" s="218"/>
-      <c r="H37" s="223"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="195"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="227"/>
-      <c r="C38" s="234"/>
-      <c r="D38" s="228"/>
-      <c r="E38" s="234" t="s">
+      <c r="B38" s="199"/>
+      <c r="C38" s="206"/>
+      <c r="D38" s="200"/>
+      <c r="E38" s="206" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="229">
+      <c r="F38" s="201">
         <f>SUM(F30:F37)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="228"/>
-      <c r="H38" s="230"/>
+      <c r="G38" s="200"/>
+      <c r="H38" s="202"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="235" t="s">
+      <c r="B40" s="218" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="236"/>
-      <c r="F40" s="237" t="s">
+      <c r="C40" s="219"/>
+      <c r="F40" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="G40" s="238"/>
-      <c r="H40" s="238"/>
+      <c r="G40" s="223"/>
+      <c r="H40" s="223"/>
     </row>
     <row r="41" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="239" t="s">
+      <c r="B41" s="220" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="221"/>
+      <c r="F41" s="220" t="s">
         <v>136</v>
       </c>
-      <c r="C41" s="240"/>
-      <c r="F41" s="239" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" s="241"/>
-      <c r="H41" s="241"/>
+      <c r="G41" s="224"/>
+      <c r="H41" s="224"/>
     </row>
     <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="242" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="243" t="s">
-        <v>173</v>
-      </c>
-      <c r="F42" s="244" t="s">
+      <c r="B42" s="207" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="208" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" s="209" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="245">
-        <v>0</v>
-      </c>
-      <c r="H42" s="246"/>
+      <c r="G42" s="214">
+        <v>0</v>
+      </c>
+      <c r="H42" s="215"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B4:H5"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="B40:C40"/>
@@ -4560,18 +4590,6 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B4:H5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -4608,45 +4626,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="234" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
+      <c r="C2" s="234"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
     </row>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="162"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
-      <c r="F3" s="164" t="s">
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="165">
+      <c r="G3" s="163">
         <f>SUM(G5:G29)*'Factor de complejidad Téc y Amb'!H9*'Factor de complejidad Téc y Amb'!H28</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="162" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="166" t="s">
+      <c r="B4" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="162" t="s">
+      <c r="D4" s="160" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="162" t="s">
+      <c r="E4" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="160" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4888,7 +4906,7 @@
       <c r="B18" s="2">
         <v>14</v>
       </c>
-      <c r="C18" s="123" t="s">
+      <c r="C18" s="121" t="s">
         <v>79</v>
       </c>
       <c r="D18" s="11"/>
@@ -4906,7 +4924,7 @@
       <c r="B19" s="2">
         <v>15</v>
       </c>
-      <c r="C19" s="123" t="s">
+      <c r="C19" s="121" t="s">
         <v>79</v>
       </c>
       <c r="D19" s="11"/>
@@ -4924,7 +4942,7 @@
       <c r="B20" s="2">
         <v>16</v>
       </c>
-      <c r="C20" s="123" t="s">
+      <c r="C20" s="121" t="s">
         <v>79</v>
       </c>
       <c r="D20" s="11"/>
@@ -5129,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5170,15 +5188,15 @@
     </row>
     <row r="2" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15"/>
-      <c r="C2" s="94" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="100">
+      <c r="C2" s="93" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="99">
         <f>'Estimación de Tamaño UCP'!G3</f>
         <v>0</v>
       </c>
-      <c r="E2" s="95" t="s">
-        <v>151</v>
+      <c r="E2" s="94" t="s">
+        <v>150</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -5194,15 +5212,15 @@
     </row>
     <row r="3" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
-      <c r="C3" s="96" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="93" t="str">
+      <c r="C3" s="95" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="92" t="str">
         <f>'Factor de complejidad Téc y Amb'!$C$42</f>
         <v>0</v>
       </c>
-      <c r="E3" s="97" t="s">
-        <v>152</v>
+      <c r="E3" s="96" t="s">
+        <v>151</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -5218,15 +5236,15 @@
     </row>
     <row r="4" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15"/>
-      <c r="C4" s="98" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="101">
+      <c r="C4" s="97" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="100">
         <f>D3*D2</f>
         <v>0</v>
       </c>
-      <c r="E4" s="99" t="s">
-        <v>152</v>
+      <c r="E4" s="98" t="s">
+        <v>151</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -5258,40 +5276,40 @@
       <c r="P5" s="16"/>
     </row>
     <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="183" t="s">
+      <c r="B6" s="238" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="184"/>
-      <c r="D6" s="184"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="184"/>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184"/>
-      <c r="J6" s="184"/>
-      <c r="K6" s="185"/>
+      <c r="C6" s="239"/>
+      <c r="D6" s="239"/>
+      <c r="E6" s="239"/>
+      <c r="F6" s="239"/>
+      <c r="G6" s="239"/>
+      <c r="H6" s="239"/>
+      <c r="I6" s="239"/>
+      <c r="J6" s="239"/>
+      <c r="K6" s="240"/>
     </row>
     <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="43"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
-      <c r="F7" s="124">
-        <f>SUM(F9+F16+F30+F46+F49)</f>
-        <v>46</v>
+      <c r="F7" s="122">
+        <f>SUM(F9+F16+F30+F47+F50)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
-      <c r="K7" s="105"/>
+      <c r="K7" s="104"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>64</v>
@@ -5300,7 +5318,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G8" s="45" t="s">
         <v>104</v>
@@ -5308,237 +5326,239 @@
       <c r="H8" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="80" t="s">
+      <c r="I8" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="81" t="s">
+      <c r="J8" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="106" t="s">
+      <c r="K8" s="105" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="138">
+      <c r="B9" s="136">
         <v>1</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="140"/>
-      <c r="E9" s="146">
+      <c r="D9" s="138"/>
+      <c r="E9" s="144" t="e">
         <f>(F9/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="149">
-        <v>0</v>
-      </c>
-      <c r="G9" s="143"/>
-      <c r="H9" s="151"/>
-      <c r="I9" s="180" t="s">
-        <v>119</v>
-      </c>
-      <c r="J9" s="181"/>
-      <c r="K9" s="145">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="147">
+        <f>SUM(F10:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="141"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="235" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" s="236"/>
+      <c r="K9" s="143">
         <f>SUM(K10:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
-      <c r="C10" s="172" t="s">
+      <c r="C10" s="170" t="s">
         <v>109</v>
       </c>
       <c r="D10" s="47"/>
-      <c r="E10" s="69"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="51">
         <v>0</v>
       </c>
       <c r="G10" s="52">
         <v>1</v>
       </c>
-      <c r="H10" s="89" t="e">
+      <c r="H10" s="88" t="e">
         <f>(F10/F9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="82" t="s">
+      <c r="I10" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="83">
+      <c r="J10" s="82">
         <f>IF(I10="Líder de proyecto",Recursos!E$5,(IF(I10="Analista",Recursos!E$6,(IF(I10="Diseñador",Recursos!#REF!,(IF(I10="Tester",Recursos!E$7,(IF(I10="Desarrollador",Recursos!E$8,(IF(I10="Arquitecto",Recursos!E$12,(IF(I10="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K10" s="108">
+      <c r="K10" s="107">
         <f t="shared" ref="K10:K15" si="0">F10*J10*G10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
-      <c r="C11" s="172" t="s">
+      <c r="C11" s="170" t="s">
         <v>110</v>
       </c>
       <c r="D11" s="47"/>
-      <c r="E11" s="69"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="51">
         <v>0</v>
       </c>
       <c r="G11" s="52">
         <v>1</v>
       </c>
-      <c r="H11" s="89" t="e">
+      <c r="H11" s="88" t="e">
         <f>(F11/F9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="82" t="s">
+      <c r="I11" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="83">
+      <c r="J11" s="82">
         <f>IF(I11="Líder de proyecto",Recursos!E$5,(IF(I11="Analista",Recursos!E$6,(IF(I11="Diseñador",Recursos!#REF!,(IF(I11="Tester",Recursos!E$7,(IF(I11="Desarrollador",Recursos!E$8,(IF(I11="Arquitecto",Recursos!E$12,(IF(I11="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K11" s="108">
+      <c r="K11" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
-      <c r="C12" s="172" t="s">
-        <v>172</v>
+      <c r="C12" s="170" t="s">
+        <v>171</v>
       </c>
       <c r="D12" s="47"/>
-      <c r="E12" s="69"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="51">
         <v>0</v>
       </c>
       <c r="G12" s="52">
         <v>1</v>
       </c>
-      <c r="H12" s="89" t="e">
+      <c r="H12" s="88" t="e">
         <f>(F12/F9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I12" s="82" t="s">
+      <c r="I12" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="83">
+      <c r="J12" s="82">
         <f>IF(I12="Líder de proyecto",Recursos!E$5,(IF(I12="Analista",Recursos!E$6,(IF(I12="Diseñador",Recursos!#REF!,(IF(I12="Tester",Recursos!E$7,(IF(I12="Desarrollador",Recursos!E$8,(IF(I12="Arquitecto",Recursos!E$12,(IF(I12="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K12" s="108">
+      <c r="K12" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
-      <c r="C13" s="172" t="s">
+      <c r="C13" s="170" t="s">
         <v>113</v>
       </c>
       <c r="D13" s="47"/>
-      <c r="E13" s="69"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="51">
         <v>0</v>
       </c>
       <c r="G13" s="52">
         <v>1</v>
       </c>
-      <c r="H13" s="89" t="e">
+      <c r="H13" s="88" t="e">
         <f>(F13/F9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="82" t="s">
+      <c r="I13" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="83">
+      <c r="J13" s="82">
         <f>IF(I13="Líder de proyecto",Recursos!E$5,(IF(I13="Analista",Recursos!E$6,(IF(I13="Diseñador",Recursos!#REF!,(IF(I13="Tester",Recursos!E$7,(IF(I13="Desarrollador",Recursos!E$8,(IF(I13="Arquitecto",Recursos!E$12,(IF(I13="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K13" s="108">
+      <c r="K13" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="47"/>
-      <c r="C14" s="172" t="s">
-        <v>177</v>
+      <c r="C14" s="170" t="s">
+        <v>176</v>
       </c>
       <c r="D14" s="47"/>
-      <c r="E14" s="69"/>
+      <c r="E14" s="68"/>
       <c r="F14" s="51">
         <v>0</v>
       </c>
       <c r="G14" s="52">
         <v>1</v>
       </c>
-      <c r="H14" s="89" t="e">
+      <c r="H14" s="88" t="e">
         <f>(F14/F9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I14" s="82" t="s">
+      <c r="I14" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="83">
+      <c r="J14" s="82">
         <f>IF(I14="Líder de proyecto",Recursos!E$5,(IF(I14="Analista",Recursos!E$6,(IF(I14="Diseñador",Recursos!#REF!,(IF(I14="Tester",Recursos!E$7,(IF(I14="Desarrollador",Recursos!E$8,(IF(I14="Arquitecto",Recursos!E$12,(IF(I14="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K14" s="108">
+      <c r="K14" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
-      <c r="C15" s="172" t="s">
+      <c r="C15" s="170" t="s">
         <v>111</v>
       </c>
       <c r="D15" s="47"/>
-      <c r="E15" s="173"/>
+      <c r="E15" s="171"/>
       <c r="F15" s="51">
         <v>0</v>
       </c>
       <c r="G15" s="52">
         <v>1</v>
       </c>
-      <c r="H15" s="89"/>
-      <c r="I15" s="82" t="s">
+      <c r="H15" s="88"/>
+      <c r="I15" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J15" s="83">
+      <c r="J15" s="82">
         <f>IF(I15="Líder de proyecto",Recursos!E$5,(IF(I15="Analista",Recursos!E$6,(IF(I15="Diseñador",Recursos!#REF!,(IF(I15="Tester",Recursos!E$7,(IF(I15="Desarrollador",Recursos!E$8,(IF(I15="Arquitecto",Recursos!E$12,(IF(I15="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K15" s="108">
+      <c r="K15" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="138">
+      <c r="B16" s="136">
         <v>2</v>
       </c>
-      <c r="C16" s="139" t="s">
+      <c r="C16" s="137" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="140"/>
-      <c r="E16" s="146">
+      <c r="D16" s="138"/>
+      <c r="E16" s="144" t="e">
         <f>(F16/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="149">
-        <v>0</v>
-      </c>
-      <c r="G16" s="143"/>
-      <c r="H16" s="151"/>
-      <c r="I16" s="187" t="s">
-        <v>120</v>
-      </c>
-      <c r="J16" s="188" t="s">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="147">
+        <f>F17+F25</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="141"/>
+      <c r="H16" s="149"/>
+      <c r="I16" s="242" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="243" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="145">
+      <c r="K16" s="143">
         <f>SUM(K17+K25)</f>
         <v>0</v>
       </c>
@@ -5548,140 +5568,141 @@
       <c r="C17" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="71"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="189" t="s">
-        <v>121</v>
-      </c>
-      <c r="J17" s="190" t="s">
+      <c r="D17" s="70"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="250">
+        <f>SUM(F18:F24)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="71"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="244" t="s">
+        <v>120</v>
+      </c>
+      <c r="J17" s="245" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="109">
+      <c r="K17" s="108">
         <f>SUM(K18:K25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
-      <c r="C18" s="172" t="s">
-        <v>178</v>
+      <c r="C18" s="170" t="s">
+        <v>177</v>
       </c>
       <c r="D18" s="47"/>
-      <c r="E18" s="69"/>
+      <c r="E18" s="68"/>
       <c r="F18" s="51">
         <v>0</v>
       </c>
       <c r="G18" s="51">
         <v>1</v>
       </c>
-      <c r="H18" s="89" t="e">
+      <c r="H18" s="88" t="e">
         <f>(F18/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I18" s="82" t="s">
+      <c r="I18" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J18" s="83">
+      <c r="J18" s="82">
         <f>IF(I18="Líder de proyecto",Recursos!E$5,(IF(I18="Analista",Recursos!E$6,(IF(I18="Diseñador",Recursos!#REF!,(IF(I18="Tester",Recursos!E$7,(IF(I18="Desarrollador",Recursos!E$8,(IF(I18="Arquitecto",Recursos!E$12,(IF(I18="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K18" s="108">
+      <c r="K18" s="107">
         <f>F18*J18*G18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="47"/>
-      <c r="C19" s="172" t="s">
-        <v>161</v>
+      <c r="C19" s="170" t="s">
+        <v>160</v>
       </c>
       <c r="D19" s="47"/>
-      <c r="E19" s="69" t="s">
-        <v>79</v>
-      </c>
+      <c r="E19" s="68"/>
       <c r="F19" s="51">
         <v>0</v>
       </c>
       <c r="G19" s="52">
         <v>1</v>
       </c>
-      <c r="H19" s="89" t="e">
+      <c r="H19" s="88" t="e">
         <f>(F19/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I19" s="82" t="s">
+      <c r="I19" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="83">
+      <c r="J19" s="82">
         <f>IF(I19="Líder de proyecto",Recursos!E$5,(IF(I19="Analista",Recursos!E$6,(IF(I19="Diseñador",Recursos!#REF!,(IF(I19="Tester",Recursos!E$7,(IF(I19="Desarrollador",Recursos!E$8,(IF(I19="Arquitecto",Recursos!E$12,(IF(I19="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K19" s="108">
+      <c r="K19" s="107">
         <f>F19*J19*G19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="47"/>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="170" t="s">
         <v>112</v>
       </c>
       <c r="D20" s="47"/>
-      <c r="E20" s="69"/>
+      <c r="E20" s="68"/>
       <c r="F20" s="51">
         <v>0</v>
       </c>
       <c r="G20" s="52">
         <v>1</v>
       </c>
-      <c r="H20" s="89" t="e">
+      <c r="H20" s="88" t="e">
         <f>(F20/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I20" s="82" t="s">
+      <c r="I20" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J20" s="83">
+      <c r="J20" s="82">
         <f>IF(I20="Líder de proyecto",Recursos!E$5,(IF(I20="Analista",Recursos!E$6,(IF(I20="Diseñador",Recursos!#REF!,(IF(I20="Tester",Recursos!E$7,(IF(I20="Desarrollador",Recursos!E$8,(IF(I20="Arquitecto",Recursos!E$12,(IF(I20="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K20" s="108">
+      <c r="K20" s="107">
         <f t="shared" ref="K20:K22" si="1">F20*J20*G20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="47"/>
-      <c r="C21" s="172" t="s">
-        <v>179</v>
+      <c r="C21" s="170" t="s">
+        <v>178</v>
       </c>
       <c r="D21" s="47"/>
-      <c r="E21" s="69"/>
+      <c r="E21" s="68"/>
       <c r="F21" s="51">
         <v>0</v>
       </c>
       <c r="G21" s="52">
         <v>1</v>
       </c>
-      <c r="H21" s="89" t="e">
+      <c r="H21" s="88" t="e">
         <f>(F21/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" s="82" t="s">
+      <c r="I21" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J21" s="83">
+      <c r="J21" s="82">
         <f>IF(I21="Líder de proyecto",Recursos!E$5,(IF(I21="Analista",Recursos!E$6,(IF(I21="Diseñador",Recursos!#REF!,(IF(I21="Tester",Recursos!E$7,(IF(I21="Desarrollador",Recursos!E$8,(IF(I21="Arquitecto",Recursos!E$12,(IF(I21="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K21" s="108">
+      <c r="K21" s="107">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N21" s="128" t="s">
+      <c r="N21" s="126" t="s">
         <v>79</v>
       </c>
       <c r="O21" s="1" t="s">
@@ -5690,90 +5711,90 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="47"/>
-      <c r="C22" s="172" t="s">
-        <v>165</v>
+      <c r="C22" s="170" t="s">
+        <v>164</v>
       </c>
       <c r="D22" s="47"/>
-      <c r="E22" s="69"/>
+      <c r="E22" s="68"/>
       <c r="F22" s="51">
         <v>0</v>
       </c>
       <c r="G22" s="52">
         <v>1</v>
       </c>
-      <c r="H22" s="89" t="e">
+      <c r="H22" s="88" t="e">
         <f>(F22/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I22" s="82" t="s">
+      <c r="I22" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J22" s="83">
+      <c r="J22" s="82">
         <f>IF(I22="Líder de proyecto",Recursos!E$5,(IF(I22="Analista",Recursos!E$6,(IF(I22="Diseñador",Recursos!#REF!,(IF(I22="Tester",Recursos!E$7,(IF(I22="Desarrollador",Recursos!E$8,(IF(I22="Arquitecto",Recursos!E$12,(IF(I22="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K22" s="108">
+      <c r="K22" s="107">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N22" s="128" t="s">
+      <c r="N22" s="126" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="47"/>
-      <c r="C23" s="172" t="s">
-        <v>180</v>
+      <c r="C23" s="170" t="s">
+        <v>179</v>
       </c>
       <c r="D23" s="47"/>
-      <c r="E23" s="69"/>
+      <c r="E23" s="68"/>
       <c r="F23" s="51">
         <v>0</v>
       </c>
       <c r="G23" s="52">
         <v>1</v>
       </c>
-      <c r="H23" s="89" t="e">
+      <c r="H23" s="88" t="e">
         <f>(F23/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I23" s="82" t="s">
+      <c r="I23" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="83">
+      <c r="J23" s="82">
         <f>IF(I23="Líder de proyecto",Recursos!E$5,(IF(I23="Analista",Recursos!E$6,(IF(I23="Diseñador",Recursos!#REF!,(IF(I23="Tester",Recursos!E$7,(IF(I23="Desarrollador",Recursos!E$8,(IF(I23="Arquitecto",Recursos!E$12,(IF(I23="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K23" s="110">
+      <c r="K23" s="109">
         <f>F23*J23*G23</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="47"/>
-      <c r="C24" s="174" t="s">
-        <v>181</v>
+      <c r="C24" s="172" t="s">
+        <v>180</v>
       </c>
       <c r="D24" s="47"/>
-      <c r="E24" s="69"/>
+      <c r="E24" s="68"/>
       <c r="F24" s="51">
         <v>0</v>
       </c>
       <c r="G24" s="52">
         <v>1</v>
       </c>
-      <c r="H24" s="89" t="e">
+      <c r="H24" s="88" t="e">
         <f>(F24/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I24" s="82" t="s">
+      <c r="I24" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="83">
+      <c r="J24" s="82">
         <f>IF(I24="Líder de proyecto",Recursos!E$5,(IF(I24="Analista",Recursos!E$6,(IF(I24="Diseñador",Recursos!#REF!,(IF(I24="Tester",Recursos!E$7,(IF(I24="Desarrollador",Recursos!E$8,(IF(I24="Arquitecto",Recursos!E$12,(IF(I24="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K24" s="110">
+      <c r="K24" s="109">
         <f>F24*J24*G24</f>
         <v>0</v>
       </c>
@@ -5783,163 +5804,166 @@
       <c r="C25" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="71"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="189" t="s">
-        <v>122</v>
-      </c>
-      <c r="J25" s="190" t="s">
+      <c r="D25" s="70"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="71">
+        <f>F27+F29</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="244" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" s="245" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="109">
+      <c r="K25" s="108">
         <f>SUM(K27:K28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="175"/>
-      <c r="C26" s="172" t="s">
-        <v>182</v>
-      </c>
-      <c r="E26" s="69"/>
+      <c r="B26" s="173"/>
+      <c r="C26" s="170" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" s="68"/>
       <c r="F26" s="51">
         <v>0</v>
       </c>
       <c r="G26" s="52">
         <v>1</v>
       </c>
-      <c r="H26" s="89" t="e">
+      <c r="H26" s="88" t="e">
         <f>(F26/F15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I26" s="82" t="s">
+      <c r="I26" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J26" s="83">
+      <c r="J26" s="82">
         <f>IF(I26="Líder de proyecto",Recursos!E$5,(IF(I26="Analista",Recursos!E$6,(IF(I26="Diseñador",Recursos!#REF!,(IF(I26="Tester",Recursos!E$7,(IF(I26="Desarrollador",Recursos!E$8,(IF(I26="Arquitecto",Recursos!E$12,(IF(I26="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K26" s="108">
+      <c r="K26" s="107">
         <f t="shared" ref="K26:K29" si="2">F26*J26*G26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="47"/>
-      <c r="C27" s="172" t="s">
-        <v>155</v>
+      <c r="C27" s="170" t="s">
+        <v>154</v>
       </c>
       <c r="D27" s="47"/>
-      <c r="E27" s="69"/>
+      <c r="E27" s="68"/>
       <c r="F27" s="51">
         <v>0</v>
       </c>
       <c r="G27" s="52">
         <v>1</v>
       </c>
-      <c r="H27" s="89" t="e">
+      <c r="H27" s="88" t="e">
         <f>(F27/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I27" s="82" t="s">
+      <c r="I27" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J27" s="83">
+      <c r="J27" s="82">
         <f>IF(I27="Líder de proyecto",Recursos!E$5,(IF(I27="Analista",Recursos!E$6,(IF(I27="Diseñador",Recursos!#REF!,(IF(I27="Tester",Recursos!E$7,(IF(I27="Desarrollador",Recursos!E$8,(IF(I27="Arquitecto",Recursos!E$12,(IF(I27="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K27" s="108">
+      <c r="K27" s="107">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="47"/>
-      <c r="C28" s="172" t="s">
-        <v>183</v>
+      <c r="C28" s="170" t="s">
+        <v>192</v>
       </c>
       <c r="D28" s="47"/>
-      <c r="E28" s="69"/>
+      <c r="E28" s="68"/>
       <c r="F28" s="51">
         <v>0</v>
       </c>
       <c r="G28" s="52">
         <v>1</v>
       </c>
-      <c r="H28" s="89" t="e">
+      <c r="H28" s="88" t="e">
         <f>(F28/F16)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="82" t="s">
+      <c r="I28" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="83">
+      <c r="J28" s="82">
         <f>IF(I28="Líder de proyecto",Recursos!E$5,(IF(I28="Analista",Recursos!E$6,(IF(I28="Diseñador",Recursos!#REF!,(IF(I28="Tester",Recursos!E$7,(IF(I28="Desarrollador",Recursos!E$8,(IF(I28="Arquitecto",Recursos!E$12,(IF(I28="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K28" s="108">
+      <c r="K28" s="107">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="47"/>
-      <c r="C29" s="172" t="s">
-        <v>156</v>
+      <c r="C29" s="170" t="s">
+        <v>155</v>
       </c>
       <c r="D29" s="47"/>
-      <c r="E29" s="173"/>
+      <c r="E29" s="171"/>
       <c r="F29" s="51">
         <v>0</v>
       </c>
       <c r="G29" s="52">
         <v>1</v>
       </c>
-      <c r="H29" s="89" t="e">
+      <c r="H29" s="88" t="e">
         <f>(F29/F17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="82" t="s">
+      <c r="I29" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J29" s="83">
+      <c r="J29" s="82">
         <f>IF(I29="Líder de proyecto",Recursos!E$5,(IF(I29="Analista",Recursos!E$6,(IF(I29="Diseñador",Recursos!#REF!,(IF(I29="Tester",Recursos!E$7,(IF(I29="Desarrollador",Recursos!E$8,(IF(I29="Arquitecto",Recursos!E$12,(IF(I29="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K29" s="108">
+      <c r="K29" s="107">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="138">
+      <c r="B30" s="136">
         <v>3</v>
       </c>
-      <c r="C30" s="139" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="147"/>
-      <c r="E30" s="148">
-        <f>SUM(E31+E36+E38+E43)</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="149">
-        <f>SUM(F31+F36+F38+F43)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="143"/>
-      <c r="H30" s="150"/>
-      <c r="I30" s="180" t="s">
-        <v>159</v>
-      </c>
-      <c r="J30" s="181" t="s">
+      <c r="C30" s="137" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="145"/>
+      <c r="E30" s="146" t="e">
+        <f>SUM(E31+E36+E38+E45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="147">
+        <f>F31+F36+F38+F45</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="141"/>
+      <c r="H30" s="148"/>
+      <c r="I30" s="235" t="s">
+        <v>158</v>
+      </c>
+      <c r="J30" s="236" t="s">
         <v>79</v>
       </c>
-      <c r="K30" s="145">
-        <f>SUM(K38+K36+K43+K31)</f>
+      <c r="K30" s="143">
+        <f>SUM(K38+K36+K44+K31)</f>
         <v>0</v>
       </c>
     </row>
@@ -5947,56 +5971,56 @@
       <c r="B31" s="54">
         <v>3.1</v>
       </c>
-      <c r="C31" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="104">
+      <c r="C31" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="59"/>
+      <c r="E31" s="103" t="e">
         <f>(F31/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="74">
-        <f>(F36*0.125)</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="70"/>
-      <c r="H31" s="84"/>
-      <c r="I31" s="191" t="s">
-        <v>170</v>
-      </c>
-      <c r="J31" s="192" t="s">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F31" s="73">
+        <f>SUM(F32:F34)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="69"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="246" t="s">
+        <v>169</v>
+      </c>
+      <c r="J31" s="247" t="s">
         <v>79</v>
       </c>
-      <c r="K31" s="107">
+      <c r="K31" s="106">
         <f>K32</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="54"/>
-      <c r="C32" s="172" t="s">
-        <v>184</v>
+      <c r="C32" s="170" t="s">
+        <v>182</v>
       </c>
       <c r="D32" s="49"/>
-      <c r="E32" s="69"/>
+      <c r="E32" s="68"/>
       <c r="F32" s="51">
         <v>0</v>
       </c>
       <c r="G32" s="56">
         <v>1</v>
       </c>
-      <c r="H32" s="89" t="e">
+      <c r="H32" s="88" t="e">
         <f>F32/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="J32" s="83">
+      <c r="I32" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="J32" s="82">
         <f>IF(I32="Líder de proyecto",Recursos!E$5,(IF(I32="Analista",Recursos!E$6,(IF(I32="Diseñador",Recursos!#REF!,(IF(I32="Tester",Recursos!E$7,(IF(I32="Desarrollador",Recursos!E$8,(IF(I32="Arquitecto",Recursos!E$12,(IF(I32="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K32" s="108">
+      <c r="K32" s="107">
         <f>F32*J32*G32</f>
         <v>0</v>
       </c>
@@ -6004,147 +6028,147 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="54"/>
-      <c r="C33" s="172" t="s">
-        <v>185</v>
+      <c r="C33" s="170" t="s">
+        <v>183</v>
       </c>
       <c r="D33" s="49"/>
-      <c r="E33" s="69"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="51">
         <v>0</v>
       </c>
       <c r="G33" s="56">
         <v>1</v>
       </c>
-      <c r="H33" s="89" t="e">
+      <c r="H33" s="88" t="e">
         <f>F33/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="J33" s="83">
+      <c r="I33" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="J33" s="82">
         <f>IF(I33="Líder de proyecto",Recursos!E$5,(IF(I33="Analista",Recursos!E$6,(IF(I33="Diseñador",Recursos!#REF!,(IF(I33="Tester",Recursos!E$7,(IF(I33="Desarrollador",Recursos!E$8,(IF(I33="Arquitecto",Recursos!E$12,(IF(I33="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K33" s="108">
+      <c r="K33" s="107">
         <f t="shared" ref="K33:K35" si="3">F33*J33*G33</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="54"/>
-      <c r="C34" s="172" t="s">
-        <v>186</v>
+      <c r="C34" s="170" t="s">
+        <v>184</v>
       </c>
       <c r="D34" s="49"/>
-      <c r="E34" s="69"/>
+      <c r="E34" s="68"/>
       <c r="F34" s="51">
         <v>0</v>
       </c>
       <c r="G34" s="56">
         <v>1</v>
       </c>
-      <c r="H34" s="89" t="e">
+      <c r="H34" s="88" t="e">
         <f>F34/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I34" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="J34" s="83">
+      <c r="I34" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="J34" s="82">
         <f>IF(I34="Líder de proyecto",Recursos!E$5,(IF(I34="Analista",Recursos!E$6,(IF(I34="Diseñador",Recursos!#REF!,(IF(I34="Tester",Recursos!E$7,(IF(I34="Desarrollador",Recursos!E$8,(IF(I34="Arquitecto",Recursos!E$12,(IF(I34="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K34" s="108">
+      <c r="K34" s="107">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="54"/>
-      <c r="C35" s="172" t="s">
-        <v>187</v>
+      <c r="C35" s="170" t="s">
+        <v>185</v>
       </c>
       <c r="D35" s="49"/>
-      <c r="E35" s="69"/>
+      <c r="E35" s="68"/>
       <c r="F35" s="51">
         <v>0</v>
       </c>
       <c r="G35" s="56">
         <v>1</v>
       </c>
-      <c r="H35" s="89" t="e">
+      <c r="H35" s="88" t="e">
         <f>F35/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="J35" s="83">
+      <c r="I35" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="J35" s="82">
         <f>IF(I35="Líder de proyecto",Recursos!E$5,(IF(I35="Analista",Recursos!E$6,(IF(I35="Diseñador",Recursos!#REF!,(IF(I35="Tester",Recursos!E$7,(IF(I35="Desarrollador",Recursos!E$8,(IF(I35="Arquitecto",Recursos!E$12,(IF(I35="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K35" s="108">
+      <c r="K35" s="107">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="54">
         <v>3.2</v>
       </c>
-      <c r="C36" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="D36" s="60"/>
-      <c r="E36" s="104">
+      <c r="C36" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="59"/>
+      <c r="E36" s="103" t="e">
         <f>(F36/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="74">
-        <f>D4</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="70"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="191" t="s">
-        <v>123</v>
-      </c>
-      <c r="J36" s="192" t="s">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F36" s="73">
+        <f>F37</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="69"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="246" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="247" t="s">
         <v>79</v>
       </c>
-      <c r="K36" s="107">
+      <c r="K36" s="106">
         <f>SUM(K37:K37)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="54"/>
       <c r="C37" s="48" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D37" s="49"/>
-      <c r="E37" s="102"/>
+      <c r="E37" s="101"/>
       <c r="F37" s="51">
         <v>0</v>
       </c>
       <c r="G37" s="56">
         <v>1</v>
       </c>
-      <c r="H37" s="89" t="e">
+      <c r="H37" s="88" t="e">
         <f>F37/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I37" s="82" t="s">
-        <v>174</v>
-      </c>
-      <c r="J37" s="83">
+      <c r="I37" s="81" t="s">
+        <v>173</v>
+      </c>
+      <c r="J37" s="82">
         <f>IF(I37="Líder de proyecto",Recursos!E$5,(IF(I37="Analista",Recursos!E$6,(IF(I37="Diseñador",Recursos!#REF!,(IF(I37="Tester",Recursos!E$7,(IF(I37="Desarrollador",Recursos!E$8,(IF(I37="Arquitecto",Recursos!E$12,(IF(I37="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K37" s="110">
+      <c r="K37" s="109">
         <f>F37*J37*G37</f>
         <v>0</v>
       </c>
@@ -6152,60 +6176,60 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="54">
         <v>3.3</v>
       </c>
-      <c r="C38" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="D38" s="63"/>
-      <c r="E38" s="104">
+      <c r="C38" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="62"/>
+      <c r="E38" s="103" t="e">
         <f>(F38/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="92">
-        <f>(F36*0.125)</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="70"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="191" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38" s="192" t="s">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F38" s="91">
+        <f>SUM(F39:F43)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="69"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="246" t="s">
+        <v>123</v>
+      </c>
+      <c r="J38" s="247" t="s">
         <v>79</v>
       </c>
-      <c r="K38" s="107">
+      <c r="K38" s="106">
         <f>SUM(K39:K42)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="54"/>
-      <c r="C39" s="48" t="s">
-        <v>162</v>
+      <c r="C39" s="170" t="s">
+        <v>161</v>
       </c>
       <c r="D39" s="50"/>
-      <c r="E39" s="69"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="51">
         <v>0</v>
       </c>
       <c r="G39" s="56">
         <v>1</v>
       </c>
-      <c r="H39" s="89" t="e">
+      <c r="H39" s="88" t="e">
         <f>F39/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I39" s="82" t="s">
+      <c r="I39" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="J39" s="83">
+      <c r="J39" s="82">
         <f>IF(I39="Líder de proyecto",Recursos!E$5,(IF(I39="Analista",Recursos!E$6,(IF(I39="Diseñador",Recursos!#REF!,(IF(I39="Tester",Recursos!E$7,(IF(I39="Desarrollador",Recursos!E$8,(IF(I39="Arquitecto",Recursos!E$12,(IF(I39="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K39" s="108">
+      <c r="K39" s="107">
         <f>F39*J39*G39</f>
         <v>0</v>
       </c>
@@ -6213,598 +6237,622 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="54"/>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="170" t="s">
         <v>116</v>
       </c>
       <c r="D40" s="50"/>
-      <c r="E40" s="69"/>
+      <c r="E40" s="68"/>
       <c r="F40" s="51">
         <v>0</v>
       </c>
       <c r="G40" s="56">
         <v>1</v>
       </c>
-      <c r="H40" s="89" t="e">
+      <c r="H40" s="88" t="e">
         <f>F40/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="82" t="s">
+      <c r="I40" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="83">
+      <c r="J40" s="82">
         <f>IF(I40="Líder de proyecto",Recursos!E$5,(IF(I40="Analista",Recursos!E$6,(IF(I40="Diseñador",Recursos!#REF!,(IF(I40="Tester",Recursos!E$7,(IF(I40="Desarrollador",Recursos!E$8,(IF(I40="Arquitecto",Recursos!E$12,(IF(I40="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K40" s="108">
+      <c r="K40" s="107">
         <f>F40*J40*G40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="54"/>
-      <c r="C41" s="48" t="s">
-        <v>117</v>
+      <c r="C41" s="170" t="s">
+        <v>159</v>
       </c>
       <c r="D41" s="50"/>
-      <c r="E41" s="69"/>
+      <c r="E41" s="68"/>
       <c r="F41" s="51">
         <v>0</v>
       </c>
       <c r="G41" s="56">
         <v>1</v>
       </c>
-      <c r="H41" s="89" t="e">
+      <c r="H41" s="88" t="e">
         <f>F41/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="82" t="s">
-        <v>174</v>
-      </c>
-      <c r="J41" s="83">
+      <c r="I41" s="81" t="s">
+        <v>173</v>
+      </c>
+      <c r="J41" s="82">
         <f>IF(I41="Líder de proyecto",Recursos!E$5,(IF(I41="Analista",Recursos!E$6,(IF(I41="Diseñador",Recursos!#REF!,(IF(I41="Tester",Recursos!E$7,(IF(I41="Desarrollador",Recursos!E$8,(IF(I41="Arquitecto",Recursos!E$12,(IF(I41="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K41" s="108">
+      <c r="K41" s="107">
         <f>F41*J41*G41</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="54"/>
-      <c r="C42" s="48" t="s">
-        <v>160</v>
+      <c r="C42" s="170" t="s">
+        <v>190</v>
       </c>
       <c r="D42" s="50"/>
-      <c r="E42" s="69"/>
+      <c r="E42" s="68"/>
       <c r="F42" s="51">
         <v>0</v>
       </c>
       <c r="G42" s="56">
         <v>1</v>
       </c>
-      <c r="H42" s="89" t="e">
+      <c r="H42" s="88" t="e">
         <f>F42/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="82" t="s">
+      <c r="I42" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="J42" s="83">
+      <c r="J42" s="82">
         <f>IF(I42="Líder de proyecto",Recursos!E$5,(IF(I42="Analista",Recursos!E$6,(IF(I42="Diseñador",Recursos!#REF!,(IF(I42="Tester",Recursos!E$7,(IF(I42="Desarrollador",Recursos!E$8,(IF(I42="Arquitecto",Recursos!E$12,(IF(I42="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K42" s="108">
+      <c r="K42" s="107">
         <f>F42*J42*G42</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="54">
+    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="253"/>
+      <c r="B43" s="251"/>
+      <c r="C43" s="170" t="s">
+        <v>191</v>
+      </c>
+      <c r="D43" s="252"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="249">
+        <v>0</v>
+      </c>
+      <c r="G43" s="254">
+        <v>1</v>
+      </c>
+      <c r="H43" s="88" t="e">
+        <f>F43/F30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="81"/>
+      <c r="J43" s="82"/>
+      <c r="K43" s="107"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="54">
         <v>3.4</v>
       </c>
-      <c r="C43" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="D43" s="61"/>
-      <c r="E43" s="104">
-        <f>(F43/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="74">
-        <f>(F36*0.2)</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="70"/>
-      <c r="H43" s="90"/>
-      <c r="I43" s="191" t="s">
-        <v>125</v>
-      </c>
-      <c r="J43" s="192" t="s">
+      <c r="C44" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="60"/>
+      <c r="E44" s="248" t="e">
+        <f>(F44/F7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F44" s="73">
+        <f>SUM(F45:F46)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="69"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="246" t="s">
+        <v>124</v>
+      </c>
+      <c r="J44" s="247" t="s">
         <v>79</v>
       </c>
-      <c r="K43" s="107">
-        <f>SUM(K44:K45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="54"/>
-      <c r="C44" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="D44" s="47"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="51">
-        <v>0</v>
-      </c>
-      <c r="G44" s="56">
-        <v>1</v>
-      </c>
-      <c r="H44" s="89">
-        <v>0.5</v>
-      </c>
-      <c r="I44" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="J44" s="83">
-        <f>IF(I44="Líder de proyecto",Recursos!E$5,(IF(I44="Analista",Recursos!E$6,(IF(I44="Diseñador",Recursos!#REF!,(IF(I44="Tester",Recursos!E$7,(IF(I44="Desarrollador",Recursos!E$8,(IF(I44="Arquitecto",Recursos!E$12,(IF(I44="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
-      </c>
-      <c r="K44" s="108">
-        <f>F44*J44*G44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K44" s="106">
+        <f>SUM(K45:K46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="54"/>
       <c r="C45" s="48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D45" s="47"/>
-      <c r="E45" s="69"/>
+      <c r="E45" s="68"/>
       <c r="F45" s="51">
         <v>0</v>
       </c>
       <c r="G45" s="56">
         <v>1</v>
       </c>
-      <c r="H45" s="89">
+      <c r="H45" s="88">
         <v>0.5</v>
       </c>
-      <c r="I45" s="82" t="s">
+      <c r="I45" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="J45" s="82">
+        <f>IF(I45="Líder de proyecto",Recursos!E$5,(IF(I45="Analista",Recursos!E$6,(IF(I45="Diseñador",Recursos!#REF!,(IF(I45="Tester",Recursos!E$7,(IF(I45="Desarrollador",Recursos!E$8,(IF(I45="Arquitecto",Recursos!E$12,(IF(I45="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>59.853275767543863</v>
+      </c>
+      <c r="K45" s="107">
+        <f>F45*J45*G45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="54"/>
+      <c r="C46" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="47"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="51">
+        <v>0</v>
+      </c>
+      <c r="G46" s="56">
+        <v>1</v>
+      </c>
+      <c r="H46" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="I46" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="J45" s="83">
-        <f>IF(I45="Líder de proyecto",Recursos!E$5,(IF(I45="Analista",Recursos!E$6,(IF(I45="Diseñador",Recursos!#REF!,(IF(I45="Tester",Recursos!E$7,(IF(I45="Desarrollador",Recursos!E$8,(IF(I45="Arquitecto",Recursos!E$12,(IF(I45="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+      <c r="J46" s="82">
+        <f>IF(I46="Líder de proyecto",Recursos!E$5,(IF(I46="Analista",Recursos!E$6,(IF(I46="Diseñador",Recursos!#REF!,(IF(I46="Tester",Recursos!E$7,(IF(I46="Desarrollador",Recursos!E$8,(IF(I46="Arquitecto",Recursos!E$12,(IF(I46="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K45" s="108">
-        <f>F45*J45*G45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="138">
+      <c r="K46" s="107">
+        <f>F46*J46*G46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="136">
         <v>4</v>
       </c>
-      <c r="C46" s="139" t="s">
+      <c r="C47" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="D46" s="140"/>
-      <c r="E46" s="146">
-        <f>(F46/F7)</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="142">
-        <f>SUM(F47:F48)</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="143"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="180" t="s">
-        <v>126</v>
-      </c>
-      <c r="J46" s="181" t="s">
+      <c r="D47" s="138"/>
+      <c r="E47" s="144" t="e">
+        <f>(F47/F7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F47" s="140">
+        <f>F48+F48</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="141"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="235" t="s">
+        <v>125</v>
+      </c>
+      <c r="J47" s="236" t="s">
         <v>79</v>
       </c>
-      <c r="K46" s="145">
-        <f>SUM(K47:K47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="47" t="s">
+      <c r="K47" s="143">
+        <f>SUM(K48:K48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="172" t="s">
-        <v>188</v>
-      </c>
-      <c r="D47" s="47"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="51">
-        <v>0</v>
-      </c>
-      <c r="G47" s="52">
-        <v>1</v>
-      </c>
-      <c r="H47" s="91">
-        <v>1</v>
-      </c>
-      <c r="I47" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="J47" s="83">
-        <f>IF(I47="Líder de proyecto",Recursos!E$5,(IF(I47="Analista",Recursos!E$6,(IF(I47="Diseñador",Recursos!#REF!,(IF(I47="Tester",Recursos!E$7,(IF(I47="Desarrollador",Recursos!E$8,(IF(I47="Arquitecto",Recursos!E$12,(IF(I47="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
-      </c>
-      <c r="K47" s="108">
-        <f>F47*J47*G47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="47"/>
-      <c r="C48" s="172" t="s">
-        <v>189</v>
+      <c r="C48" s="170" t="s">
+        <v>186</v>
       </c>
       <c r="D48" s="47"/>
-      <c r="E48" s="176"/>
+      <c r="E48" s="174"/>
       <c r="F48" s="51">
         <v>0</v>
       </c>
       <c r="G48" s="52">
         <v>1</v>
       </c>
-      <c r="H48" s="91">
+      <c r="H48" s="90">
         <v>1</v>
       </c>
-      <c r="I48" s="82"/>
-      <c r="J48" s="83"/>
-      <c r="K48" s="108"/>
+      <c r="I48" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="J48" s="82">
+        <f>IF(I48="Líder de proyecto",Recursos!E$5,(IF(I48="Analista",Recursos!E$6,(IF(I48="Diseñador",Recursos!#REF!,(IF(I48="Tester",Recursos!E$7,(IF(I48="Desarrollador",Recursos!E$8,(IF(I48="Arquitecto",Recursos!E$12,(IF(I48="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>59.853275767543863</v>
+      </c>
+      <c r="K48" s="107">
+        <f>F48*J48*G48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="138">
+      <c r="B49" s="47"/>
+      <c r="C49" s="170" t="s">
+        <v>187</v>
+      </c>
+      <c r="D49" s="47"/>
+      <c r="E49" s="174"/>
+      <c r="F49" s="51">
+        <v>0</v>
+      </c>
+      <c r="G49" s="52">
+        <v>1</v>
+      </c>
+      <c r="H49" s="90">
+        <v>1</v>
+      </c>
+      <c r="I49" s="81"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="107"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="136">
         <v>5</v>
       </c>
-      <c r="C49" s="139" t="s">
+      <c r="C50" s="137" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="138"/>
+      <c r="E50" s="139" t="e">
+        <f>(F50/F7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F50" s="140">
+        <f>SUM(F51:F54)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="141"/>
+      <c r="H50" s="142"/>
+      <c r="I50" s="235" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="140"/>
-      <c r="E49" s="141">
-        <f>(F49/F7)</f>
+      <c r="J50" s="236" t="s">
+        <v>79</v>
+      </c>
+      <c r="K50" s="143">
+        <f>SUM(K51:K54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="63"/>
+      <c r="C51" s="114" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="115"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="117">
+        <v>0</v>
+      </c>
+      <c r="G51" s="118">
         <v>1</v>
       </c>
-      <c r="F49" s="142">
-        <f>SUM(F50:F53)</f>
-        <v>46</v>
-      </c>
-      <c r="G49" s="143"/>
-      <c r="H49" s="144"/>
-      <c r="I49" s="180" t="s">
-        <v>135</v>
-      </c>
-      <c r="J49" s="181" t="s">
-        <v>79</v>
-      </c>
-      <c r="K49" s="145">
-        <f>SUM(K50:K53)</f>
-        <v>1749.7255208333333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="64"/>
-      <c r="C50" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="D50" s="116"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="118">
-        <v>12</v>
-      </c>
-      <c r="G50" s="119">
-        <v>1</v>
-      </c>
-      <c r="H50" s="125">
-        <f>(F50/F49)</f>
-        <v>0.2608695652173913</v>
-      </c>
-      <c r="I50" s="82" t="s">
-        <v>176</v>
-      </c>
-      <c r="J50" s="83">
-        <f>IF(I50="Líder de proyecto",Recursos!E$5,(IF(I50="Analista",Recursos!E$6,(IF(I50="Administrador de la configuración",Recursos!E$11,(IF(I50="Tester",Recursos!E$7,(IF(I50="Desarrollador",Recursos!E$8,(IF(I50="Arquitecto",Recursos!E$12,(IF(I50="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+      <c r="H51" s="123" t="e">
+        <f>(F51/F50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="J51" s="82">
+        <f>IF(I51="Líder de proyecto",Recursos!E$5,(IF(I51="Analista",Recursos!E$6,(IF(I51="Administrador de la configuración",Recursos!E$11,(IF(I51="Tester",Recursos!E$7,(IF(I51="Desarrollador",Recursos!E$8,(IF(I51="Arquitecto",Recursos!E$12,(IF(I51="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>31.977576754385964</v>
       </c>
-      <c r="K50" s="120">
-        <f>F50*J50*G50</f>
-        <v>383.73092105263157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="115" t="s">
-        <v>127</v>
-      </c>
-      <c r="D51" s="116"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="118">
-        <v>24</v>
-      </c>
-      <c r="G51" s="119">
-        <v>1</v>
-      </c>
-      <c r="H51" s="125">
-        <f>(F51/F49)</f>
-        <v>0.52173913043478259</v>
-      </c>
-      <c r="I51" s="82" t="s">
-        <v>175</v>
-      </c>
-      <c r="J51" s="83">
-        <f>IF(I51="Líder de proyecto",Recursos!E$5,(IF(I51="Analista",Recursos!E$6,(IF(I51="Diseñador",Recursos!#REF!,(IF(I51="Tester",Recursos!E$7,(IF(I51="Desarrollador",Recursos!E$8,(IF(I51="Arquitecto",Recursos!E$12,(IF(I51="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
-        <v>31.977576754385964</v>
-      </c>
-      <c r="K51" s="120">
+      <c r="K51" s="119">
         <f>F51*J51*G51</f>
-        <v>767.46184210526314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="115" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="116"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="118">
-        <v>4</v>
-      </c>
-      <c r="G52" s="119">
+      <c r="C52" s="114" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="115"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="117">
+        <v>0</v>
+      </c>
+      <c r="G52" s="118">
         <v>1</v>
       </c>
-      <c r="H52" s="125">
-        <f>(F52/F49)</f>
-        <v>8.6956521739130432E-2</v>
-      </c>
-      <c r="I52" s="82" t="s">
+      <c r="H52" s="123" t="e">
+        <f>(F52/F50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" s="81" t="s">
+        <v>174</v>
+      </c>
+      <c r="J52" s="82">
+        <f>IF(I52="Líder de proyecto",Recursos!E$5,(IF(I52="Analista",Recursos!E$6,(IF(I52="Diseñador",Recursos!#REF!,(IF(I52="Tester",Recursos!E$7,(IF(I52="Desarrollador",Recursos!E$8,(IF(I52="Arquitecto",Recursos!E$12,(IF(I52="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>31.977576754385964</v>
+      </c>
+      <c r="K52" s="119">
+        <f>F52*J52*G52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="114" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="115"/>
+      <c r="E53" s="68"/>
+      <c r="F53" s="117">
+        <v>0</v>
+      </c>
+      <c r="G53" s="118">
+        <v>1</v>
+      </c>
+      <c r="H53" s="123" t="e">
+        <f>(F53/F50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="J52" s="83">
-        <f>IF(I52="Líder de proyecto",Recursos!E$5,(IF(I52="Analista",Recursos!E$6,(IF(I52="Diseñador",Recursos!#REF!,(IF(I52="Tester",Recursos!E$7,(IF(I52="Desarrollador",Recursos!E$8,(IF(I52="Arquitecto",Recursos!E$12,(IF(I52="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
-      </c>
-      <c r="K52" s="120">
-        <f>F52*J52*G52</f>
-        <v>239.41310307017545</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="103" t="s">
-        <v>79</v>
-      </c>
-      <c r="C53" s="117" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="116"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="121">
-        <v>6</v>
-      </c>
-      <c r="G53" s="122">
-        <v>1</v>
-      </c>
-      <c r="H53" s="125">
-        <f>(F53/F49)</f>
-        <v>0.13043478260869565</v>
-      </c>
-      <c r="I53" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="J53" s="83">
+      <c r="J53" s="82">
         <f>IF(I53="Líder de proyecto",Recursos!E$5,(IF(I53="Analista",Recursos!E$6,(IF(I53="Diseñador",Recursos!#REF!,(IF(I53="Tester",Recursos!E$7,(IF(I53="Desarrollador",Recursos!E$8,(IF(I53="Arquitecto",Recursos!E$12,(IF(I53="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K53" s="120">
+      <c r="K53" s="119">
         <f>F53*J53*G53</f>
-        <v>359.11965460526318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="130">
+      <c r="B54" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="115"/>
+      <c r="E54" s="68"/>
+      <c r="F54" s="117">
+        <v>0</v>
+      </c>
+      <c r="G54" s="120">
+        <v>1</v>
+      </c>
+      <c r="H54" s="123" t="e">
+        <f>(F54/F50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="J54" s="82">
+        <f>IF(I54="Líder de proyecto",Recursos!E$5,(IF(I54="Analista",Recursos!E$6,(IF(I54="Diseñador",Recursos!#REF!,(IF(I54="Tester",Recursos!E$7,(IF(I54="Desarrollador",Recursos!E$8,(IF(I54="Arquitecto",Recursos!E$12,(IF(I54="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>59.853275767543863</v>
+      </c>
+      <c r="K54" s="119">
+        <f>F54*J54*G54</f>
+        <v>0</v>
+      </c>
+      <c r="L54" s="81"/>
+    </row>
+    <row r="55" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="128">
         <v>6</v>
       </c>
-      <c r="C54" s="131" t="s">
+      <c r="C55" s="129" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" s="130"/>
+      <c r="E55" s="131"/>
+      <c r="F55" s="132">
+        <v>6</v>
+      </c>
+      <c r="G55" s="133">
+        <v>1</v>
+      </c>
+      <c r="H55" s="134" t="s">
+        <v>79</v>
+      </c>
+      <c r="I55" s="235" t="s">
         <v>153</v>
       </c>
-      <c r="D54" s="132"/>
-      <c r="E54" s="133"/>
-      <c r="F54" s="134" t="s">
+      <c r="J55" s="236"/>
+      <c r="K55" s="135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="87"/>
+      <c r="F56" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G54" s="135">
-        <v>1</v>
-      </c>
-      <c r="H54" s="136" t="s">
-        <v>79</v>
-      </c>
-      <c r="I54" s="180" t="s">
-        <v>154</v>
-      </c>
-      <c r="J54" s="181"/>
-      <c r="K54" s="137">
-        <v>0</v>
-      </c>
-      <c r="L54" s="82"/>
-    </row>
-    <row r="55" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="186" t="s">
-        <v>118</v>
-      </c>
-      <c r="J55" s="186"/>
-      <c r="K55" s="75">
-        <f>SUM(K49+K46+K30+K16+K9+K54)</f>
-        <v>1749.7255208333333</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B56" s="129"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="17"/>
-      <c r="I56" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="J56" s="156"/>
-      <c r="K56" s="157">
-        <f>(200*F7)-K55</f>
-        <v>7450.2744791666664</v>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="241" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" s="241"/>
+      <c r="K56" s="74">
+        <f>SUM(K50+K47+K30+K16+K9+K55)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="B57" s="127"/>
       <c r="C57" s="55"/>
       <c r="D57" s="17"/>
-      <c r="I57" s="152" t="s">
+      <c r="I57" s="153" t="s">
         <v>146</v>
       </c>
-      <c r="J57" s="153"/>
-      <c r="K57" s="154" t="s">
-        <v>79</v>
+      <c r="J57" s="154"/>
+      <c r="K57" s="155">
+        <f>(200*F7)-K56</f>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C58" s="55"/>
       <c r="D58" s="17"/>
-      <c r="I58" s="152"/>
-      <c r="J58" s="153"/>
-      <c r="K58" s="154">
-        <v>0</v>
+      <c r="I58" s="150" t="s">
+        <v>145</v>
+      </c>
+      <c r="J58" s="151"/>
+      <c r="K58" s="152" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C59" s="55"/>
       <c r="D59" s="17"/>
-      <c r="I59" s="152"/>
-      <c r="J59" s="153"/>
-      <c r="K59" s="154">
+      <c r="I59" s="150"/>
+      <c r="J59" s="151"/>
+      <c r="K59" s="152">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C60" s="55"/>
       <c r="D60" s="17"/>
-      <c r="I60" s="152"/>
-      <c r="J60" s="153"/>
-      <c r="K60" s="154">
+      <c r="I60" s="150"/>
+      <c r="J60" s="151"/>
+      <c r="K60" s="152">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C61" s="55"/>
       <c r="D61" s="17"/>
-      <c r="I61" s="152"/>
-      <c r="J61" s="153"/>
-      <c r="K61" s="154">
+      <c r="I61" s="150"/>
+      <c r="J61" s="151"/>
+      <c r="K61" s="152">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C62" s="55"/>
       <c r="D62" s="17"/>
-      <c r="I62" s="86" t="s">
+      <c r="I62" s="150"/>
+      <c r="J62" s="151"/>
+      <c r="K62" s="152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="C63" s="55"/>
+      <c r="D63" s="17"/>
+      <c r="I63" s="85" t="s">
+        <v>142</v>
+      </c>
+      <c r="J63" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="J62" s="86" t="s">
+      <c r="K63" s="86">
+        <f>SUM(K56:K62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="237"/>
+      <c r="D64" s="237"/>
+      <c r="I64" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K64" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="I65" s="85" t="s">
+        <v>142</v>
+      </c>
+      <c r="J65" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="K62" s="87">
-        <f>SUM(K55:K61)</f>
-        <v>9200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="182"/>
-      <c r="D63" s="182"/>
-      <c r="I63" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K63" s="1">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I64" s="86" t="s">
-        <v>143</v>
-      </c>
-      <c r="J64" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="K64" s="85">
-        <f>K62*K63</f>
-        <v>10672</v>
-      </c>
-    </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C65" s="9" t="s">
+      <c r="K65" s="84">
+        <f>K63*K64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C66" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I65" s="53" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I66" s="53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="126" t="s">
+    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I67" s="53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="124" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="C64:D64"/>
     <mergeCell ref="B6:K6"/>
-    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="I56:J56"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I47:J47"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I55:J55"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G50:G54 G44:G45 G39:G42 G37 G26:G29 G10:G15 G19:G24 G32:G35 G47:G48">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51:G55 G45:G46 G37 G26:G29 G10:G15 G19:G24 G32:G35 G48:G49 G39:G43">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51:I53 I10:I15 I18:I24 I26:I29 I37 I39:I42 I44:I45 I47:I48 I32:I35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I52:I54 I10:I15 I18:I24 I26:I29 I37 I45:I46 I48:I49 I32:I35 I39:I43">
       <formula1>"Líder de proyecto, Analista, Arquitecto, Tester, Desarrollador, Aseguramiento de la calidad"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51">
       <formula1>"Líder de proyecto, Analista, Arquitecto, Tester, Desarrollador,Administrador de la configuración, Aseguramiento de la calidad"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6812,7 +6860,7 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="K36 K38 K43 K46 K49" formula="1"/>
+    <ignoredError sqref="K36 K38 K44 K47 K50" formula="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -6841,233 +6889,233 @@
     </row>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="156" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="158" t="s">
+      <c r="D4" s="156" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="159" t="s">
+      <c r="E4" s="157" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="112" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="75">
         <v>11788.65</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="75">
         <f>C5/30.4/8</f>
         <v>48.473067434210527</v>
       </c>
-      <c r="E5" s="77">
+      <c r="E5" s="76">
         <f t="shared" ref="E5:E12" si="0">SUM(D5+E$27)</f>
         <v>59.853275767543863</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="75">
         <v>9785.6299999999992</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="75">
         <f t="shared" ref="D6:D12" si="1">C6/30.4/8</f>
         <v>40.236965460526314</v>
       </c>
-      <c r="E6" s="77">
+      <c r="E6" s="76">
         <f t="shared" si="0"/>
         <v>51.617173793859649</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="112" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="75">
         <v>9785.6299999999992</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="75">
         <f t="shared" si="1"/>
         <v>40.236965460526314</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="76">
         <f t="shared" si="0"/>
         <v>51.617173793859649</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="127" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="76">
+      <c r="B8" s="125" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="75">
         <v>11788.65</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="75">
         <f t="shared" si="1"/>
         <v>48.473067434210527</v>
       </c>
-      <c r="E8" s="77">
+      <c r="E8" s="76">
         <f t="shared" si="0"/>
         <v>59.853275767543863</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="127" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="76">
+      <c r="B9" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="75">
         <v>5009.28</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="75">
         <f t="shared" si="1"/>
         <v>20.597368421052632</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="76">
         <f t="shared" si="0"/>
         <v>31.977576754385964</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="75">
         <v>9176.4599999999991</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="75">
         <f t="shared" si="1"/>
         <v>37.732154605263155</v>
       </c>
-      <c r="E10" s="77">
+      <c r="E10" s="76">
         <f t="shared" si="0"/>
         <v>49.11236293859649</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="127" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" s="76">
+      <c r="B11" s="125" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="75">
         <v>5009.28</v>
       </c>
-      <c r="D11" s="76">
+      <c r="D11" s="75">
         <f t="shared" ref="D11" si="2">C11/30.4/8</f>
         <v>20.597368421052632</v>
       </c>
-      <c r="E11" s="77">
+      <c r="E11" s="76">
         <f t="shared" si="0"/>
         <v>31.977576754385964</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="114" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="76">
+      <c r="B12" s="113" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="75">
         <v>11788.65</v>
       </c>
-      <c r="D12" s="111">
+      <c r="D12" s="110">
         <f t="shared" si="1"/>
         <v>48.473067434210527</v>
       </c>
-      <c r="E12" s="112">
+      <c r="E12" s="111">
         <f t="shared" si="0"/>
         <v>59.853275767543863</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="160" t="s">
+      <c r="B15" s="158" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="66" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="77">
+      <c r="C16" s="76">
         <v>2800</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="77">
+      <c r="C17" s="76">
         <v>1600</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="76">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="76">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="76">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="76">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="C18" s="77">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="77">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="66" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="77">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="77">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="66" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="77">
+      <c r="C22" s="76">
         <v>1800</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="78">
+      <c r="C23" s="77">
         <f>SUM(C16:C22)</f>
         <v>21850</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="161" t="s">
+      <c r="B27" s="159" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="64">
         <v>8</v>
       </c>
-      <c r="D27" s="161" t="s">
+      <c r="D27" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="79">
+      <c r="E27" s="78">
         <f>((C23/C27)/30/8)</f>
         <v>11.380208333333334</v>
       </c>
@@ -7078,34 +7126,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
-    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -7189,39 +7209,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
+    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7236,4 +7252,36 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualizacion de informacion en PTLL_estimacion esfuerzo
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/2. Estimación y Planeación/Plantillas estimación/PTLL_Estimación_Esfuerzo.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/2. Estimación y Planeación/Plantillas estimación/PTLL_Estimación_Esfuerzo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Ciclo de vida IWM\2. Estimación y Planeación\Plantillas estimación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\Procesos\Ciclo de vida IWM\2. Estimación y Planeación\Plantillas estimación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1588,7 +1588,7 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1825,9 +1825,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="30" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="30" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1902,7 +1900,6 @@
     <xf numFmtId="9" fontId="45" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="43" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2101,11 +2098,74 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="25" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2115,14 +2175,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2151,42 +2203,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2229,25 +2245,13 @@
     <xf numFmtId="0" fontId="34" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="27" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3103,28 +3107,28 @@
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="168" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="167"/>
-      <c r="B2" s="212" t="s">
+    <row r="2" spans="1:7" s="165" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="164"/>
+      <c r="B2" s="216" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="212"/>
-      <c r="D2" s="213" t="s">
+      <c r="C2" s="216"/>
+      <c r="D2" s="217" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
-    </row>
-    <row r="4" spans="1:7" s="166" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="165"/>
-      <c r="B4" s="169" t="s">
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+    </row>
+    <row r="4" spans="1:7" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="162"/>
+      <c r="B4" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="165"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -3163,15 +3167,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="166" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="165"/>
-      <c r="B12" s="169" t="s">
+    <row r="12" spans="1:7" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="162"/>
+      <c r="B12" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="165"/>
-      <c r="E12" s="165"/>
-      <c r="F12" s="165"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="162"/>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
@@ -3305,15 +3309,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:256" s="166" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A31" s="165"/>
-      <c r="B31" s="169" t="s">
+    <row r="31" spans="1:256" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="162"/>
+      <c r="B31" s="166" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="165"/>
-      <c r="D31" s="165"/>
-      <c r="E31" s="165"/>
-      <c r="F31" s="165"/>
+      <c r="C31" s="162"/>
+      <c r="D31" s="162"/>
+      <c r="E31" s="162"/>
+      <c r="F31" s="162"/>
     </row>
     <row r="32" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
@@ -3934,646 +3938,634 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="182" customWidth="1"/>
-    <col min="2" max="2" width="15" style="182" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="182" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="182" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="182" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="182" customWidth="1"/>
-    <col min="7" max="7" width="46.140625" style="182" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="182" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="182"/>
+    <col min="1" max="1" width="5.28515625" style="179" customWidth="1"/>
+    <col min="2" max="2" width="15" style="179" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" style="179" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="179" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="179" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="179" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" style="179" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="179" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="179"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="178" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="232" t="s">
+      <c r="B3" s="218" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
+      <c r="C3" s="218"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="218"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="218"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="233" t="s">
+      <c r="B4" s="226" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="233"/>
-      <c r="D4" s="233"/>
-      <c r="E4" s="233"/>
-      <c r="F4" s="233"/>
-      <c r="G4" s="233"/>
-      <c r="H4" s="233"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="233"/>
-      <c r="C5" s="233"/>
-      <c r="D5" s="233"/>
-      <c r="E5" s="233"/>
-      <c r="F5" s="233"/>
-      <c r="G5" s="233"/>
-      <c r="H5" s="233"/>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
     </row>
     <row r="8" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="227" t="s">
+      <c r="B8" s="221" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="228"/>
-      <c r="D8" s="228"/>
-      <c r="E8" s="228"/>
-      <c r="F8" s="228"/>
-      <c r="G8" s="228"/>
-      <c r="H8" s="229"/>
+      <c r="C8" s="222"/>
+      <c r="D8" s="222"/>
+      <c r="E8" s="222"/>
+      <c r="F8" s="222"/>
+      <c r="G8" s="222"/>
+      <c r="H8" s="223"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="183"/>
-      <c r="C9" s="184"/>
-      <c r="D9" s="184"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="184" t="s">
+      <c r="B9" s="180"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="185">
+      <c r="H9" s="182">
         <f>0.6+(0.01*SUM(F11:F23))</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="186" t="s">
+      <c r="B10" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="187" t="s">
+      <c r="C10" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="188" t="s">
+      <c r="D10" s="185" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="188" t="s">
+      <c r="E10" s="185" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="186" t="s">
+      <c r="F10" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="230" t="s">
+      <c r="G10" s="224" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="231"/>
+      <c r="H10" s="225"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="189" t="s">
+      <c r="B11" s="186" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="190" t="s">
+      <c r="C11" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="175">
+      <c r="D11" s="172">
         <v>2</v>
       </c>
-      <c r="E11" s="191">
-        <v>0</v>
-      </c>
-      <c r="F11" s="178">
+      <c r="E11" s="188">
+        <v>0</v>
+      </c>
+      <c r="F11" s="175">
         <f t="shared" ref="F11:F23" si="0">E11*D11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="225"/>
-      <c r="H11" s="226"/>
-      <c r="K11" s="192"/>
+      <c r="G11" s="227"/>
+      <c r="H11" s="228"/>
+      <c r="K11" s="189"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="193" t="s">
+      <c r="B12" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="192" t="s">
+      <c r="C12" s="189" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="176">
+      <c r="D12" s="173">
         <v>2</v>
       </c>
-      <c r="E12" s="194">
-        <v>0</v>
-      </c>
-      <c r="F12" s="179">
+      <c r="E12" s="191">
+        <v>0</v>
+      </c>
+      <c r="F12" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="216"/>
-      <c r="H12" s="217"/>
+      <c r="G12" s="219"/>
+      <c r="H12" s="220"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="193" t="s">
+      <c r="B13" s="190" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="192" t="s">
+      <c r="C13" s="189" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="176">
+      <c r="D13" s="173">
         <v>1</v>
       </c>
-      <c r="E13" s="194">
-        <v>0</v>
-      </c>
-      <c r="F13" s="179">
+      <c r="E13" s="191">
+        <v>0</v>
+      </c>
+      <c r="F13" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="216"/>
-      <c r="H13" s="217"/>
+      <c r="G13" s="219"/>
+      <c r="H13" s="220"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="193" t="s">
+      <c r="B14" s="190" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="192" t="s">
+      <c r="C14" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="176">
+      <c r="D14" s="173">
         <v>1</v>
       </c>
-      <c r="E14" s="194">
-        <v>0</v>
-      </c>
-      <c r="F14" s="179">
+      <c r="E14" s="191">
+        <v>0</v>
+      </c>
+      <c r="F14" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="216"/>
-      <c r="H14" s="217"/>
+      <c r="G14" s="219"/>
+      <c r="H14" s="220"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="193" t="s">
+      <c r="B15" s="190" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="192" t="s">
+      <c r="C15" s="189" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="176">
+      <c r="D15" s="173">
         <v>1</v>
       </c>
-      <c r="E15" s="194">
-        <v>0</v>
-      </c>
-      <c r="F15" s="179">
+      <c r="E15" s="191">
+        <v>0</v>
+      </c>
+      <c r="F15" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="216"/>
-      <c r="H15" s="217"/>
+      <c r="G15" s="219"/>
+      <c r="H15" s="220"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="193" t="s">
+      <c r="B16" s="190" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="192" t="s">
+      <c r="C16" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="176">
+      <c r="D16" s="173">
         <v>0.5</v>
       </c>
-      <c r="E16" s="194">
-        <v>0</v>
-      </c>
-      <c r="F16" s="179">
+      <c r="E16" s="191">
+        <v>0</v>
+      </c>
+      <c r="F16" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="192"/>
-      <c r="H16" s="195"/>
+      <c r="G16" s="189"/>
+      <c r="H16" s="192"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="193" t="s">
+      <c r="B17" s="190" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="192" t="s">
+      <c r="C17" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="176">
+      <c r="D17" s="173">
         <v>0.5</v>
       </c>
-      <c r="E17" s="194">
-        <v>0</v>
-      </c>
-      <c r="F17" s="179">
+      <c r="E17" s="191">
+        <v>0</v>
+      </c>
+      <c r="F17" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="216"/>
-      <c r="H17" s="217"/>
+      <c r="G17" s="219"/>
+      <c r="H17" s="220"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="193" t="s">
+      <c r="B18" s="190" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="192" t="s">
+      <c r="C18" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="176">
+      <c r="D18" s="173">
         <v>2</v>
       </c>
-      <c r="E18" s="194">
-        <v>0</v>
-      </c>
-      <c r="F18" s="179">
+      <c r="E18" s="191">
+        <v>0</v>
+      </c>
+      <c r="F18" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="192"/>
-      <c r="H18" s="195"/>
+      <c r="G18" s="189"/>
+      <c r="H18" s="192"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="193" t="s">
+      <c r="B19" s="190" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="192" t="s">
+      <c r="C19" s="189" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="176">
+      <c r="D19" s="173">
         <v>1</v>
       </c>
-      <c r="E19" s="194">
-        <v>0</v>
-      </c>
-      <c r="F19" s="179">
+      <c r="E19" s="191">
+        <v>0</v>
+      </c>
+      <c r="F19" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="216"/>
-      <c r="H19" s="217"/>
+      <c r="G19" s="219"/>
+      <c r="H19" s="220"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="193" t="s">
+      <c r="B20" s="190" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="192" t="s">
+      <c r="C20" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="176">
+      <c r="D20" s="173">
         <v>1</v>
       </c>
-      <c r="E20" s="194">
-        <v>0</v>
-      </c>
-      <c r="F20" s="179">
+      <c r="E20" s="191">
+        <v>0</v>
+      </c>
+      <c r="F20" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="216"/>
-      <c r="H20" s="217"/>
+      <c r="G20" s="219"/>
+      <c r="H20" s="220"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="193" t="s">
+      <c r="B21" s="190" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="192" t="s">
+      <c r="C21" s="189" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="176">
+      <c r="D21" s="173">
         <v>1</v>
       </c>
-      <c r="E21" s="194">
-        <v>0</v>
-      </c>
-      <c r="F21" s="179">
+      <c r="E21" s="191">
+        <v>0</v>
+      </c>
+      <c r="F21" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="216"/>
-      <c r="H21" s="217"/>
+      <c r="G21" s="219"/>
+      <c r="H21" s="220"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="193" t="s">
+      <c r="B22" s="190" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="192" t="s">
+      <c r="C22" s="189" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="176">
+      <c r="D22" s="173">
         <v>1</v>
       </c>
-      <c r="E22" s="194">
-        <v>0</v>
-      </c>
-      <c r="F22" s="179">
+      <c r="E22" s="191">
+        <v>0</v>
+      </c>
+      <c r="F22" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="216"/>
-      <c r="H22" s="217"/>
+      <c r="G22" s="219"/>
+      <c r="H22" s="220"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="196" t="s">
+      <c r="B23" s="193" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="197" t="s">
+      <c r="C23" s="194" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="177">
+      <c r="D23" s="174">
         <v>1</v>
       </c>
-      <c r="E23" s="198">
-        <v>0</v>
-      </c>
-      <c r="F23" s="180">
+      <c r="E23" s="195">
+        <v>0</v>
+      </c>
+      <c r="F23" s="177">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="216"/>
-      <c r="H23" s="217"/>
+      <c r="G23" s="219"/>
+      <c r="H23" s="220"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="199"/>
-      <c r="C24" s="200"/>
-      <c r="D24" s="200"/>
-      <c r="E24" s="200" t="s">
+      <c r="B24" s="196"/>
+      <c r="C24" s="197"/>
+      <c r="D24" s="197"/>
+      <c r="E24" s="197" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="201">
+      <c r="F24" s="198">
         <f>SUM(F11:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="200"/>
-      <c r="H24" s="202"/>
+      <c r="G24" s="197"/>
+      <c r="H24" s="199"/>
     </row>
     <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="227" t="s">
+      <c r="B27" s="221" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="228"/>
-      <c r="D27" s="228"/>
-      <c r="E27" s="228"/>
-      <c r="F27" s="228"/>
-      <c r="G27" s="228"/>
-      <c r="H27" s="229"/>
+      <c r="C27" s="222"/>
+      <c r="D27" s="222"/>
+      <c r="E27" s="222"/>
+      <c r="F27" s="222"/>
+      <c r="G27" s="222"/>
+      <c r="H27" s="223"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B28" s="184"/>
-      <c r="C28" s="184"/>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="184"/>
-      <c r="G28" s="184" t="s">
+      <c r="B28" s="181"/>
+      <c r="C28" s="181"/>
+      <c r="D28" s="181"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="181"/>
+      <c r="G28" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="184">
+      <c r="H28" s="181">
         <f>1.4+(-0.03*SUM(F30:F37))</f>
         <v>1.4</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="186" t="s">
+      <c r="B29" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="187" t="s">
+      <c r="C29" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="188" t="s">
+      <c r="D29" s="185" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="188" t="s">
+      <c r="E29" s="185" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="186" t="s">
+      <c r="F29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="230" t="s">
+      <c r="G29" s="224" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="231"/>
+      <c r="H29" s="225"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="189" t="s">
+      <c r="B30" s="186" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="203" t="s">
+      <c r="C30" s="200" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="210">
+      <c r="D30" s="207">
         <v>1.5</v>
       </c>
-      <c r="E30" s="191">
-        <v>0</v>
-      </c>
-      <c r="F30" s="204">
+      <c r="E30" s="188">
+        <v>0</v>
+      </c>
+      <c r="F30" s="201">
         <f t="shared" ref="F30:F37" si="1">E30*D30</f>
         <v>0</v>
       </c>
-      <c r="G30" s="225"/>
-      <c r="H30" s="226"/>
+      <c r="G30" s="227"/>
+      <c r="H30" s="228"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="193" t="s">
+      <c r="B31" s="190" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="192" t="s">
+      <c r="C31" s="189" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="211">
+      <c r="D31" s="208">
         <v>0.5</v>
       </c>
-      <c r="E31" s="194">
-        <v>0</v>
-      </c>
-      <c r="F31" s="205">
+      <c r="E31" s="191">
+        <v>0</v>
+      </c>
+      <c r="F31" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G31" s="216"/>
-      <c r="H31" s="217"/>
+      <c r="G31" s="219"/>
+      <c r="H31" s="220"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="193" t="s">
+      <c r="B32" s="190" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="192" t="s">
+      <c r="C32" s="189" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="211">
+      <c r="D32" s="208">
         <v>1</v>
       </c>
-      <c r="E32" s="194">
-        <v>0</v>
-      </c>
-      <c r="F32" s="205">
+      <c r="E32" s="191">
+        <v>0</v>
+      </c>
+      <c r="F32" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="216"/>
-      <c r="H32" s="217"/>
+      <c r="G32" s="219"/>
+      <c r="H32" s="220"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="193" t="s">
+      <c r="B33" s="190" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="192" t="s">
+      <c r="C33" s="189" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="211">
+      <c r="D33" s="208">
         <v>0.5</v>
       </c>
-      <c r="E33" s="194">
-        <v>0</v>
-      </c>
-      <c r="F33" s="205">
+      <c r="E33" s="191">
+        <v>0</v>
+      </c>
+      <c r="F33" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G33" s="216"/>
-      <c r="H33" s="217"/>
+      <c r="G33" s="219"/>
+      <c r="H33" s="220"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="193" t="s">
+      <c r="B34" s="190" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="192" t="s">
+      <c r="C34" s="189" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="211">
+      <c r="D34" s="208">
         <v>1</v>
       </c>
-      <c r="E34" s="194">
-        <v>0</v>
-      </c>
-      <c r="F34" s="205">
+      <c r="E34" s="191">
+        <v>0</v>
+      </c>
+      <c r="F34" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G34" s="216"/>
-      <c r="H34" s="217"/>
+      <c r="G34" s="219"/>
+      <c r="H34" s="220"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="193" t="s">
+      <c r="B35" s="190" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="192" t="s">
+      <c r="C35" s="189" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="211">
+      <c r="D35" s="208">
         <v>2</v>
       </c>
-      <c r="E35" s="194">
-        <v>0</v>
-      </c>
-      <c r="F35" s="205">
+      <c r="E35" s="191">
+        <v>0</v>
+      </c>
+      <c r="F35" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G35" s="192"/>
-      <c r="H35" s="195"/>
+      <c r="G35" s="189"/>
+      <c r="H35" s="192"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="193" t="s">
+      <c r="B36" s="190" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="192" t="s">
+      <c r="C36" s="189" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="211">
+      <c r="D36" s="208">
         <v>-1</v>
       </c>
-      <c r="E36" s="194">
-        <v>0</v>
-      </c>
-      <c r="F36" s="205">
+      <c r="E36" s="191">
+        <v>0</v>
+      </c>
+      <c r="F36" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36" s="216"/>
-      <c r="H36" s="217"/>
+      <c r="G36" s="219"/>
+      <c r="H36" s="220"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="193" t="s">
+      <c r="B37" s="190" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="192" t="s">
+      <c r="C37" s="189" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="211">
+      <c r="D37" s="208">
         <v>2</v>
       </c>
-      <c r="E37" s="194">
-        <v>0</v>
-      </c>
-      <c r="F37" s="205">
+      <c r="E37" s="191">
+        <v>0</v>
+      </c>
+      <c r="F37" s="202">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G37" s="192"/>
-      <c r="H37" s="195"/>
+      <c r="G37" s="189"/>
+      <c r="H37" s="192"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="199"/>
-      <c r="C38" s="206"/>
-      <c r="D38" s="200"/>
-      <c r="E38" s="206" t="s">
+      <c r="B38" s="196"/>
+      <c r="C38" s="203"/>
+      <c r="D38" s="197"/>
+      <c r="E38" s="203" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="201">
+      <c r="F38" s="198">
         <f>SUM(F30:F37)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="200"/>
-      <c r="H38" s="202"/>
+      <c r="G38" s="197"/>
+      <c r="H38" s="199"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="218" t="s">
+      <c r="B40" s="231" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="219"/>
-      <c r="F40" s="222" t="s">
+      <c r="C40" s="232"/>
+      <c r="F40" s="235" t="s">
         <v>66</v>
       </c>
-      <c r="G40" s="223"/>
-      <c r="H40" s="223"/>
+      <c r="G40" s="236"/>
+      <c r="H40" s="236"/>
     </row>
     <row r="41" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="220" t="s">
+      <c r="B41" s="233" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="221"/>
-      <c r="F41" s="220" t="s">
+      <c r="C41" s="234"/>
+      <c r="F41" s="233" t="s">
         <v>136</v>
       </c>
-      <c r="G41" s="224"/>
-      <c r="H41" s="224"/>
+      <c r="G41" s="237"/>
+      <c r="H41" s="237"/>
     </row>
     <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="207" t="s">
+      <c r="B42" s="204" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="208" t="s">
+      <c r="C42" s="205" t="s">
         <v>172</v>
       </c>
-      <c r="F42" s="209" t="s">
+      <c r="F42" s="206" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="214">
-        <v>0</v>
-      </c>
-      <c r="H42" s="215"/>
+      <c r="G42" s="229">
+        <v>0</v>
+      </c>
+      <c r="H42" s="230"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B4:H5"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="B40:C40"/>
@@ -4590,6 +4582,18 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B4:H5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -4626,45 +4630,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="234" t="s">
+      <c r="B2" s="238" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="234"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="234"/>
-      <c r="F2" s="234"/>
-      <c r="G2" s="234"/>
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="238"/>
+      <c r="F2" s="238"/>
+      <c r="G2" s="238"/>
     </row>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="160"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="163">
+      <c r="G3" s="160">
         <f>SUM(G5:G29)*'Factor de complejidad Téc y Amb'!H9*'Factor de complejidad Téc y Amb'!H28</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="164" t="s">
+      <c r="B4" s="157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="160" t="s">
+      <c r="D4" s="157" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="160" t="s">
+      <c r="E4" s="157" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="160" t="s">
+      <c r="F4" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="160" t="s">
+      <c r="G4" s="157" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4906,7 +4910,7 @@
       <c r="B18" s="2">
         <v>14</v>
       </c>
-      <c r="C18" s="121" t="s">
+      <c r="C18" s="119" t="s">
         <v>79</v>
       </c>
       <c r="D18" s="11"/>
@@ -4924,7 +4928,7 @@
       <c r="B19" s="2">
         <v>15</v>
       </c>
-      <c r="C19" s="121" t="s">
+      <c r="C19" s="119" t="s">
         <v>79</v>
       </c>
       <c r="D19" s="11"/>
@@ -4942,7 +4946,7 @@
       <c r="B20" s="2">
         <v>16</v>
       </c>
-      <c r="C20" s="121" t="s">
+      <c r="C20" s="119" t="s">
         <v>79</v>
       </c>
       <c r="D20" s="11"/>
@@ -5149,8 +5153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5276,25 +5280,25 @@
       <c r="P5" s="16"/>
     </row>
     <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="238" t="s">
+      <c r="B6" s="242" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="239"/>
-      <c r="D6" s="239"/>
-      <c r="E6" s="239"/>
-      <c r="F6" s="239"/>
-      <c r="G6" s="239"/>
-      <c r="H6" s="239"/>
-      <c r="I6" s="239"/>
-      <c r="J6" s="239"/>
-      <c r="K6" s="240"/>
+      <c r="C6" s="243"/>
+      <c r="D6" s="243"/>
+      <c r="E6" s="243"/>
+      <c r="F6" s="243"/>
+      <c r="G6" s="243"/>
+      <c r="H6" s="243"/>
+      <c r="I6" s="243"/>
+      <c r="J6" s="243"/>
+      <c r="K6" s="244"/>
     </row>
     <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="43"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
-      <c r="F7" s="122">
+      <c r="F7" s="120">
         <f>SUM(F9+F16+F30+F47+F50)</f>
         <v>0</v>
       </c>
@@ -5337,35 +5341,35 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="136">
+      <c r="B9" s="134">
         <v>1</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="C9" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="138"/>
-      <c r="E9" s="144" t="e">
+      <c r="D9" s="136"/>
+      <c r="E9" s="141" t="e">
         <f>(F9/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F9" s="147">
+      <c r="F9" s="144">
         <f>SUM(F10:F15)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="141"/>
-      <c r="H9" s="149"/>
-      <c r="I9" s="235" t="s">
+      <c r="G9" s="139"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="239" t="s">
         <v>118</v>
       </c>
-      <c r="J9" s="236"/>
-      <c r="K9" s="143">
+      <c r="J9" s="240"/>
+      <c r="K9" s="252">
         <f>SUM(K10:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
-      <c r="C10" s="170" t="s">
+      <c r="C10" s="167" t="s">
         <v>109</v>
       </c>
       <c r="D10" s="47"/>
@@ -5387,14 +5391,14 @@
         <f>IF(I10="Líder de proyecto",Recursos!E$5,(IF(I10="Analista",Recursos!E$6,(IF(I10="Diseñador",Recursos!#REF!,(IF(I10="Tester",Recursos!E$7,(IF(I10="Desarrollador",Recursos!E$8,(IF(I10="Arquitecto",Recursos!E$12,(IF(I10="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K10" s="107">
+      <c r="K10" s="106">
         <f t="shared" ref="K10:K15" si="0">F10*J10*G10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
-      <c r="C11" s="170" t="s">
+      <c r="C11" s="167" t="s">
         <v>110</v>
       </c>
       <c r="D11" s="47"/>
@@ -5416,14 +5420,14 @@
         <f>IF(I11="Líder de proyecto",Recursos!E$5,(IF(I11="Analista",Recursos!E$6,(IF(I11="Diseñador",Recursos!#REF!,(IF(I11="Tester",Recursos!E$7,(IF(I11="Desarrollador",Recursos!E$8,(IF(I11="Arquitecto",Recursos!E$12,(IF(I11="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K11" s="107">
+      <c r="K11" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
-      <c r="C12" s="170" t="s">
+      <c r="C12" s="167" t="s">
         <v>171</v>
       </c>
       <c r="D12" s="47"/>
@@ -5445,14 +5449,14 @@
         <f>IF(I12="Líder de proyecto",Recursos!E$5,(IF(I12="Analista",Recursos!E$6,(IF(I12="Diseñador",Recursos!#REF!,(IF(I12="Tester",Recursos!E$7,(IF(I12="Desarrollador",Recursos!E$8,(IF(I12="Arquitecto",Recursos!E$12,(IF(I12="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K12" s="107">
+      <c r="K12" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
-      <c r="C13" s="170" t="s">
+      <c r="C13" s="167" t="s">
         <v>113</v>
       </c>
       <c r="D13" s="47"/>
@@ -5474,14 +5478,14 @@
         <f>IF(I13="Líder de proyecto",Recursos!E$5,(IF(I13="Analista",Recursos!E$6,(IF(I13="Diseñador",Recursos!#REF!,(IF(I13="Tester",Recursos!E$7,(IF(I13="Desarrollador",Recursos!E$8,(IF(I13="Arquitecto",Recursos!E$12,(IF(I13="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K13" s="107">
+      <c r="K13" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="47"/>
-      <c r="C14" s="170" t="s">
+      <c r="C14" s="167" t="s">
         <v>176</v>
       </c>
       <c r="D14" s="47"/>
@@ -5503,18 +5507,18 @@
         <f>IF(I14="Líder de proyecto",Recursos!E$5,(IF(I14="Analista",Recursos!E$6,(IF(I14="Diseñador",Recursos!#REF!,(IF(I14="Tester",Recursos!E$7,(IF(I14="Desarrollador",Recursos!E$8,(IF(I14="Arquitecto",Recursos!E$12,(IF(I14="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K14" s="107">
+      <c r="K14" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
-      <c r="C15" s="170" t="s">
+      <c r="C15" s="167" t="s">
         <v>111</v>
       </c>
       <c r="D15" s="47"/>
-      <c r="E15" s="171"/>
+      <c r="E15" s="168"/>
       <c r="F15" s="51">
         <v>0</v>
       </c>
@@ -5529,36 +5533,36 @@
         <f>IF(I15="Líder de proyecto",Recursos!E$5,(IF(I15="Analista",Recursos!E$6,(IF(I15="Diseñador",Recursos!#REF!,(IF(I15="Tester",Recursos!E$7,(IF(I15="Desarrollador",Recursos!E$8,(IF(I15="Arquitecto",Recursos!E$12,(IF(I15="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K15" s="107">
+      <c r="K15" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="136">
+      <c r="B16" s="134">
         <v>2</v>
       </c>
-      <c r="C16" s="137" t="s">
+      <c r="C16" s="135" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="138"/>
-      <c r="E16" s="144" t="e">
+      <c r="D16" s="136"/>
+      <c r="E16" s="141" t="e">
         <f>(F16/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F16" s="147">
+      <c r="F16" s="144">
         <f>F17+F25</f>
         <v>0</v>
       </c>
-      <c r="G16" s="141"/>
-      <c r="H16" s="149"/>
-      <c r="I16" s="242" t="s">
+      <c r="G16" s="139"/>
+      <c r="H16" s="146"/>
+      <c r="I16" s="246" t="s">
         <v>119</v>
       </c>
-      <c r="J16" s="243" t="s">
+      <c r="J16" s="247" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="143">
+      <c r="K16" s="252">
         <f>SUM(K17+K25)</f>
         <v>0</v>
       </c>
@@ -5570,26 +5574,26 @@
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="68"/>
-      <c r="F17" s="250">
+      <c r="F17" s="211">
         <f>SUM(F18:F24)</f>
         <v>0</v>
       </c>
       <c r="G17" s="71"/>
       <c r="H17" s="72"/>
-      <c r="I17" s="244" t="s">
+      <c r="I17" s="248" t="s">
         <v>120</v>
       </c>
-      <c r="J17" s="245" t="s">
+      <c r="J17" s="249" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="108">
+      <c r="K17" s="253">
         <f>SUM(K18:K25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
-      <c r="C18" s="170" t="s">
+      <c r="C18" s="167" t="s">
         <v>177</v>
       </c>
       <c r="D18" s="47"/>
@@ -5611,14 +5615,14 @@
         <f>IF(I18="Líder de proyecto",Recursos!E$5,(IF(I18="Analista",Recursos!E$6,(IF(I18="Diseñador",Recursos!#REF!,(IF(I18="Tester",Recursos!E$7,(IF(I18="Desarrollador",Recursos!E$8,(IF(I18="Arquitecto",Recursos!E$12,(IF(I18="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K18" s="107">
+      <c r="K18" s="106">
         <f>F18*J18*G18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="47"/>
-      <c r="C19" s="170" t="s">
+      <c r="C19" s="167" t="s">
         <v>160</v>
       </c>
       <c r="D19" s="47"/>
@@ -5640,14 +5644,14 @@
         <f>IF(I19="Líder de proyecto",Recursos!E$5,(IF(I19="Analista",Recursos!E$6,(IF(I19="Diseñador",Recursos!#REF!,(IF(I19="Tester",Recursos!E$7,(IF(I19="Desarrollador",Recursos!E$8,(IF(I19="Arquitecto",Recursos!E$12,(IF(I19="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K19" s="107">
+      <c r="K19" s="106">
         <f>F19*J19*G19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="47"/>
-      <c r="C20" s="170" t="s">
+      <c r="C20" s="167" t="s">
         <v>112</v>
       </c>
       <c r="D20" s="47"/>
@@ -5669,14 +5673,14 @@
         <f>IF(I20="Líder de proyecto",Recursos!E$5,(IF(I20="Analista",Recursos!E$6,(IF(I20="Diseñador",Recursos!#REF!,(IF(I20="Tester",Recursos!E$7,(IF(I20="Desarrollador",Recursos!E$8,(IF(I20="Arquitecto",Recursos!E$12,(IF(I20="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K20" s="107">
+      <c r="K20" s="106">
         <f t="shared" ref="K20:K22" si="1">F20*J20*G20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="47"/>
-      <c r="C21" s="170" t="s">
+      <c r="C21" s="167" t="s">
         <v>178</v>
       </c>
       <c r="D21" s="47"/>
@@ -5698,11 +5702,11 @@
         <f>IF(I21="Líder de proyecto",Recursos!E$5,(IF(I21="Analista",Recursos!E$6,(IF(I21="Diseñador",Recursos!#REF!,(IF(I21="Tester",Recursos!E$7,(IF(I21="Desarrollador",Recursos!E$8,(IF(I21="Arquitecto",Recursos!E$12,(IF(I21="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K21" s="107">
+      <c r="K21" s="106">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N21" s="126" t="s">
+      <c r="N21" s="124" t="s">
         <v>79</v>
       </c>
       <c r="O21" s="1" t="s">
@@ -5711,7 +5715,7 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="47"/>
-      <c r="C22" s="170" t="s">
+      <c r="C22" s="167" t="s">
         <v>164</v>
       </c>
       <c r="D22" s="47"/>
@@ -5733,17 +5737,17 @@
         <f>IF(I22="Líder de proyecto",Recursos!E$5,(IF(I22="Analista",Recursos!E$6,(IF(I22="Diseñador",Recursos!#REF!,(IF(I22="Tester",Recursos!E$7,(IF(I22="Desarrollador",Recursos!E$8,(IF(I22="Arquitecto",Recursos!E$12,(IF(I22="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K22" s="107">
+      <c r="K22" s="106">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N22" s="126" t="s">
+      <c r="N22" s="124" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="47"/>
-      <c r="C23" s="170" t="s">
+      <c r="C23" s="167" t="s">
         <v>179</v>
       </c>
       <c r="D23" s="47"/>
@@ -5765,14 +5769,14 @@
         <f>IF(I23="Líder de proyecto",Recursos!E$5,(IF(I23="Analista",Recursos!E$6,(IF(I23="Diseñador",Recursos!#REF!,(IF(I23="Tester",Recursos!E$7,(IF(I23="Desarrollador",Recursos!E$8,(IF(I23="Arquitecto",Recursos!E$12,(IF(I23="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K23" s="109">
+      <c r="K23" s="107">
         <f>F23*J23*G23</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="47"/>
-      <c r="C24" s="172" t="s">
+      <c r="C24" s="169" t="s">
         <v>180</v>
       </c>
       <c r="D24" s="47"/>
@@ -5794,7 +5798,7 @@
         <f>IF(I24="Líder de proyecto",Recursos!E$5,(IF(I24="Analista",Recursos!E$6,(IF(I24="Diseñador",Recursos!#REF!,(IF(I24="Tester",Recursos!E$7,(IF(I24="Desarrollador",Recursos!E$8,(IF(I24="Arquitecto",Recursos!E$12,(IF(I24="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K24" s="109">
+      <c r="K24" s="107">
         <f>F24*J24*G24</f>
         <v>0</v>
       </c>
@@ -5806,26 +5810,26 @@
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="68"/>
-      <c r="F25" s="71">
-        <f>F27+F29</f>
+      <c r="F25" s="254">
+        <f>SUM(F26:F29)</f>
         <v>0</v>
       </c>
       <c r="G25" s="71"/>
       <c r="H25" s="72"/>
-      <c r="I25" s="244" t="s">
+      <c r="I25" s="248" t="s">
         <v>121</v>
       </c>
-      <c r="J25" s="245" t="s">
+      <c r="J25" s="249" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="108">
+      <c r="K25" s="253">
         <f>SUM(K27:K28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="173"/>
-      <c r="C26" s="170" t="s">
+      <c r="B26" s="170"/>
+      <c r="C26" s="167" t="s">
         <v>181</v>
       </c>
       <c r="E26" s="68"/>
@@ -5846,14 +5850,14 @@
         <f>IF(I26="Líder de proyecto",Recursos!E$5,(IF(I26="Analista",Recursos!E$6,(IF(I26="Diseñador",Recursos!#REF!,(IF(I26="Tester",Recursos!E$7,(IF(I26="Desarrollador",Recursos!E$8,(IF(I26="Arquitecto",Recursos!E$12,(IF(I26="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K26" s="107">
+      <c r="K26" s="106">
         <f t="shared" ref="K26:K29" si="2">F26*J26*G26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="47"/>
-      <c r="C27" s="170" t="s">
+      <c r="C27" s="167" t="s">
         <v>154</v>
       </c>
       <c r="D27" s="47"/>
@@ -5875,14 +5879,14 @@
         <f>IF(I27="Líder de proyecto",Recursos!E$5,(IF(I27="Analista",Recursos!E$6,(IF(I27="Diseñador",Recursos!#REF!,(IF(I27="Tester",Recursos!E$7,(IF(I27="Desarrollador",Recursos!E$8,(IF(I27="Arquitecto",Recursos!E$12,(IF(I27="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K27" s="107">
+      <c r="K27" s="106">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="47"/>
-      <c r="C28" s="170" t="s">
+      <c r="C28" s="167" t="s">
         <v>192</v>
       </c>
       <c r="D28" s="47"/>
@@ -5904,18 +5908,18 @@
         <f>IF(I28="Líder de proyecto",Recursos!E$5,(IF(I28="Analista",Recursos!E$6,(IF(I28="Diseñador",Recursos!#REF!,(IF(I28="Tester",Recursos!E$7,(IF(I28="Desarrollador",Recursos!E$8,(IF(I28="Arquitecto",Recursos!E$12,(IF(I28="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K28" s="107">
+      <c r="K28" s="106">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="47"/>
-      <c r="C29" s="170" t="s">
+      <c r="C29" s="167" t="s">
         <v>155</v>
       </c>
       <c r="D29" s="47"/>
-      <c r="E29" s="171"/>
+      <c r="E29" s="168"/>
       <c r="F29" s="51">
         <v>0</v>
       </c>
@@ -5933,36 +5937,36 @@
         <f>IF(I29="Líder de proyecto",Recursos!E$5,(IF(I29="Analista",Recursos!E$6,(IF(I29="Diseñador",Recursos!#REF!,(IF(I29="Tester",Recursos!E$7,(IF(I29="Desarrollador",Recursos!E$8,(IF(I29="Arquitecto",Recursos!E$12,(IF(I29="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K29" s="107">
+      <c r="K29" s="106">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="136">
+      <c r="B30" s="134">
         <v>3</v>
       </c>
-      <c r="C30" s="137" t="s">
+      <c r="C30" s="135" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="145"/>
-      <c r="E30" s="146" t="e">
+      <c r="D30" s="142"/>
+      <c r="E30" s="143" t="e">
         <f>SUM(E31+E36+E38+E45)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F30" s="147">
+      <c r="F30" s="144">
         <f>F31+F36+F38+F45</f>
         <v>0</v>
       </c>
-      <c r="G30" s="141"/>
-      <c r="H30" s="148"/>
-      <c r="I30" s="235" t="s">
+      <c r="G30" s="139"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="239" t="s">
         <v>158</v>
       </c>
-      <c r="J30" s="236" t="s">
+      <c r="J30" s="240" t="s">
         <v>79</v>
       </c>
-      <c r="K30" s="143">
+      <c r="K30" s="252">
         <f>SUM(K38+K36+K44+K31)</f>
         <v>0</v>
       </c>
@@ -5980,25 +5984,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F31" s="73">
-        <f>SUM(F32:F34)</f>
+        <f>SUM(F32:F35)</f>
         <v>0</v>
       </c>
       <c r="G31" s="69"/>
       <c r="H31" s="83"/>
-      <c r="I31" s="246" t="s">
+      <c r="I31" s="250" t="s">
         <v>169</v>
       </c>
-      <c r="J31" s="247" t="s">
+      <c r="J31" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="K31" s="106">
+      <c r="K31" s="255">
         <f>K32</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="54"/>
-      <c r="C32" s="170" t="s">
+      <c r="C32" s="167" t="s">
         <v>182</v>
       </c>
       <c r="D32" s="49"/>
@@ -6020,7 +6024,7 @@
         <f>IF(I32="Líder de proyecto",Recursos!E$5,(IF(I32="Analista",Recursos!E$6,(IF(I32="Diseñador",Recursos!#REF!,(IF(I32="Tester",Recursos!E$7,(IF(I32="Desarrollador",Recursos!E$8,(IF(I32="Arquitecto",Recursos!E$12,(IF(I32="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K32" s="107">
+      <c r="K32" s="106">
         <f>F32*J32*G32</f>
         <v>0</v>
       </c>
@@ -6030,7 +6034,7 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="54"/>
-      <c r="C33" s="170" t="s">
+      <c r="C33" s="167" t="s">
         <v>183</v>
       </c>
       <c r="D33" s="49"/>
@@ -6052,14 +6056,14 @@
         <f>IF(I33="Líder de proyecto",Recursos!E$5,(IF(I33="Analista",Recursos!E$6,(IF(I33="Diseñador",Recursos!#REF!,(IF(I33="Tester",Recursos!E$7,(IF(I33="Desarrollador",Recursos!E$8,(IF(I33="Arquitecto",Recursos!E$12,(IF(I33="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K33" s="107">
+      <c r="K33" s="106">
         <f t="shared" ref="K33:K35" si="3">F33*J33*G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="54"/>
-      <c r="C34" s="170" t="s">
+      <c r="C34" s="167" t="s">
         <v>184</v>
       </c>
       <c r="D34" s="49"/>
@@ -6081,14 +6085,14 @@
         <f>IF(I34="Líder de proyecto",Recursos!E$5,(IF(I34="Analista",Recursos!E$6,(IF(I34="Diseñador",Recursos!#REF!,(IF(I34="Tester",Recursos!E$7,(IF(I34="Desarrollador",Recursos!E$8,(IF(I34="Arquitecto",Recursos!E$12,(IF(I34="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K34" s="107">
+      <c r="K34" s="106">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="54"/>
-      <c r="C35" s="170" t="s">
+      <c r="C35" s="167" t="s">
         <v>185</v>
       </c>
       <c r="D35" s="49"/>
@@ -6110,7 +6114,7 @@
         <f>IF(I35="Líder de proyecto",Recursos!E$5,(IF(I35="Analista",Recursos!E$6,(IF(I35="Diseñador",Recursos!#REF!,(IF(I35="Tester",Recursos!E$7,(IF(I35="Desarrollador",Recursos!E$8,(IF(I35="Arquitecto",Recursos!E$12,(IF(I35="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K35" s="107">
+      <c r="K35" s="106">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6133,13 +6137,13 @@
       </c>
       <c r="G36" s="69"/>
       <c r="H36" s="61"/>
-      <c r="I36" s="246" t="s">
+      <c r="I36" s="250" t="s">
         <v>122</v>
       </c>
-      <c r="J36" s="247" t="s">
+      <c r="J36" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="K36" s="106">
+      <c r="K36" s="255">
         <f>SUM(K37:K37)</f>
         <v>0</v>
       </c>
@@ -6168,7 +6172,7 @@
         <f>IF(I37="Líder de proyecto",Recursos!E$5,(IF(I37="Analista",Recursos!E$6,(IF(I37="Diseñador",Recursos!#REF!,(IF(I37="Tester",Recursos!E$7,(IF(I37="Desarrollador",Recursos!E$8,(IF(I37="Arquitecto",Recursos!E$12,(IF(I37="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K37" s="109">
+      <c r="K37" s="107">
         <f>F37*J37*G37</f>
         <v>0</v>
       </c>
@@ -6194,20 +6198,20 @@
       </c>
       <c r="G38" s="69"/>
       <c r="H38" s="61"/>
-      <c r="I38" s="246" t="s">
+      <c r="I38" s="250" t="s">
         <v>123</v>
       </c>
-      <c r="J38" s="247" t="s">
+      <c r="J38" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="K38" s="106">
+      <c r="K38" s="255">
         <f>SUM(K39:K42)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="54"/>
-      <c r="C39" s="170" t="s">
+      <c r="C39" s="167" t="s">
         <v>161</v>
       </c>
       <c r="D39" s="50"/>
@@ -6229,7 +6233,7 @@
         <f>IF(I39="Líder de proyecto",Recursos!E$5,(IF(I39="Analista",Recursos!E$6,(IF(I39="Diseñador",Recursos!#REF!,(IF(I39="Tester",Recursos!E$7,(IF(I39="Desarrollador",Recursos!E$8,(IF(I39="Arquitecto",Recursos!E$12,(IF(I39="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K39" s="107">
+      <c r="K39" s="106">
         <f>F39*J39*G39</f>
         <v>0</v>
       </c>
@@ -6239,7 +6243,7 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="54"/>
-      <c r="C40" s="170" t="s">
+      <c r="C40" s="167" t="s">
         <v>116</v>
       </c>
       <c r="D40" s="50"/>
@@ -6261,14 +6265,14 @@
         <f>IF(I40="Líder de proyecto",Recursos!E$5,(IF(I40="Analista",Recursos!E$6,(IF(I40="Diseñador",Recursos!#REF!,(IF(I40="Tester",Recursos!E$7,(IF(I40="Desarrollador",Recursos!E$8,(IF(I40="Arquitecto",Recursos!E$12,(IF(I40="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K40" s="107">
+      <c r="K40" s="106">
         <f>F40*J40*G40</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="54"/>
-      <c r="C41" s="170" t="s">
+      <c r="C41" s="167" t="s">
         <v>159</v>
       </c>
       <c r="D41" s="50"/>
@@ -6290,14 +6294,14 @@
         <f>IF(I41="Líder de proyecto",Recursos!E$5,(IF(I41="Analista",Recursos!E$6,(IF(I41="Diseñador",Recursos!#REF!,(IF(I41="Tester",Recursos!E$7,(IF(I41="Desarrollador",Recursos!E$8,(IF(I41="Arquitecto",Recursos!E$12,(IF(I41="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K41" s="107">
+      <c r="K41" s="106">
         <f>F41*J41*G41</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="54"/>
-      <c r="C42" s="170" t="s">
+      <c r="C42" s="167" t="s">
         <v>190</v>
       </c>
       <c r="D42" s="50"/>
@@ -6319,23 +6323,23 @@
         <f>IF(I42="Líder de proyecto",Recursos!E$5,(IF(I42="Analista",Recursos!E$6,(IF(I42="Diseñador",Recursos!#REF!,(IF(I42="Tester",Recursos!E$7,(IF(I42="Desarrollador",Recursos!E$8,(IF(I42="Arquitecto",Recursos!E$12,(IF(I42="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K42" s="107">
+      <c r="K42" s="106">
         <f>F42*J42*G42</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="253"/>
-      <c r="B43" s="251"/>
-      <c r="C43" s="170" t="s">
+      <c r="A43" s="214"/>
+      <c r="B43" s="212"/>
+      <c r="C43" s="167" t="s">
         <v>191</v>
       </c>
-      <c r="D43" s="252"/>
+      <c r="D43" s="213"/>
       <c r="E43" s="68"/>
-      <c r="F43" s="249">
-        <v>0</v>
-      </c>
-      <c r="G43" s="254">
+      <c r="F43" s="210">
+        <v>0</v>
+      </c>
+      <c r="G43" s="215">
         <v>1</v>
       </c>
       <c r="H43" s="88" t="e">
@@ -6344,7 +6348,7 @@
       </c>
       <c r="I43" s="81"/>
       <c r="J43" s="82"/>
-      <c r="K43" s="107"/>
+      <c r="K43" s="106"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="54">
@@ -6354,7 +6358,7 @@
         <v>168</v>
       </c>
       <c r="D44" s="60"/>
-      <c r="E44" s="248" t="e">
+      <c r="E44" s="209" t="e">
         <f>(F44/F7)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6364,13 +6368,13 @@
       </c>
       <c r="G44" s="69"/>
       <c r="H44" s="89"/>
-      <c r="I44" s="246" t="s">
+      <c r="I44" s="250" t="s">
         <v>124</v>
       </c>
-      <c r="J44" s="247" t="s">
+      <c r="J44" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="K44" s="106">
+      <c r="K44" s="255">
         <f>SUM(K45:K46)</f>
         <v>0</v>
       </c>
@@ -6398,7 +6402,7 @@
         <f>IF(I45="Líder de proyecto",Recursos!E$5,(IF(I45="Analista",Recursos!E$6,(IF(I45="Diseñador",Recursos!#REF!,(IF(I45="Tester",Recursos!E$7,(IF(I45="Desarrollador",Recursos!E$8,(IF(I45="Arquitecto",Recursos!E$12,(IF(I45="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K45" s="107">
+      <c r="K45" s="106">
         <f>F45*J45*G45</f>
         <v>0</v>
       </c>
@@ -6426,36 +6430,36 @@
         <f>IF(I46="Líder de proyecto",Recursos!E$5,(IF(I46="Analista",Recursos!E$6,(IF(I46="Diseñador",Recursos!#REF!,(IF(I46="Tester",Recursos!E$7,(IF(I46="Desarrollador",Recursos!E$8,(IF(I46="Arquitecto",Recursos!E$12,(IF(I46="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K46" s="107">
+      <c r="K46" s="106">
         <f>F46*J46*G46</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="136">
+      <c r="B47" s="134">
         <v>4</v>
       </c>
-      <c r="C47" s="137" t="s">
+      <c r="C47" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="138"/>
-      <c r="E47" s="144" t="e">
+      <c r="D47" s="136"/>
+      <c r="E47" s="141" t="e">
         <f>(F47/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F47" s="140">
-        <f>F48+F48</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="141"/>
-      <c r="H47" s="142"/>
-      <c r="I47" s="235" t="s">
+      <c r="F47" s="138">
+        <f>F48+F49</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="139"/>
+      <c r="H47" s="140"/>
+      <c r="I47" s="239" t="s">
         <v>125</v>
       </c>
-      <c r="J47" s="236" t="s">
+      <c r="J47" s="240" t="s">
         <v>79</v>
       </c>
-      <c r="K47" s="143">
+      <c r="K47" s="252">
         <f>SUM(K48:K48)</f>
         <v>0</v>
       </c>
@@ -6464,11 +6468,11 @@
       <c r="B48" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="170" t="s">
+      <c r="C48" s="167" t="s">
         <v>186</v>
       </c>
       <c r="D48" s="47"/>
-      <c r="E48" s="174"/>
+      <c r="E48" s="171"/>
       <c r="F48" s="51">
         <v>0</v>
       </c>
@@ -6485,18 +6489,18 @@
         <f>IF(I48="Líder de proyecto",Recursos!E$5,(IF(I48="Analista",Recursos!E$6,(IF(I48="Diseñador",Recursos!#REF!,(IF(I48="Tester",Recursos!E$7,(IF(I48="Desarrollador",Recursos!E$8,(IF(I48="Arquitecto",Recursos!E$12,(IF(I48="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K48" s="107">
+      <c r="K48" s="106">
         <f>F48*J48*G48</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="47"/>
-      <c r="C49" s="170" t="s">
+      <c r="C49" s="167" t="s">
         <v>187</v>
       </c>
       <c r="D49" s="47"/>
-      <c r="E49" s="174"/>
+      <c r="E49" s="171"/>
       <c r="F49" s="51">
         <v>0</v>
       </c>
@@ -6508,51 +6512,51 @@
       </c>
       <c r="I49" s="81"/>
       <c r="J49" s="82"/>
-      <c r="K49" s="107"/>
+      <c r="K49" s="106"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="136">
+      <c r="B50" s="134">
         <v>5</v>
       </c>
-      <c r="C50" s="137" t="s">
+      <c r="C50" s="135" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="138"/>
-      <c r="E50" s="139" t="e">
+      <c r="D50" s="136"/>
+      <c r="E50" s="137" t="e">
         <f>(F50/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F50" s="140">
+      <c r="F50" s="138">
         <f>SUM(F51:F54)</f>
         <v>0</v>
       </c>
-      <c r="G50" s="141"/>
-      <c r="H50" s="142"/>
-      <c r="I50" s="235" t="s">
+      <c r="G50" s="139"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="239" t="s">
         <v>134</v>
       </c>
-      <c r="J50" s="236" t="s">
+      <c r="J50" s="240" t="s">
         <v>79</v>
       </c>
-      <c r="K50" s="143">
+      <c r="K50" s="252">
         <f>SUM(K51:K54)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="63"/>
-      <c r="C51" s="114" t="s">
+      <c r="C51" s="112" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="115"/>
+      <c r="D51" s="113"/>
       <c r="E51" s="68"/>
-      <c r="F51" s="117">
-        <v>0</v>
-      </c>
-      <c r="G51" s="118">
+      <c r="F51" s="115">
+        <v>0</v>
+      </c>
+      <c r="G51" s="116">
         <v>1</v>
       </c>
-      <c r="H51" s="123" t="e">
+      <c r="H51" s="121" t="e">
         <f>(F51/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6563,7 +6567,7 @@
         <f>IF(I51="Líder de proyecto",Recursos!E$5,(IF(I51="Analista",Recursos!E$6,(IF(I51="Administrador de la configuración",Recursos!E$11,(IF(I51="Tester",Recursos!E$7,(IF(I51="Desarrollador",Recursos!E$8,(IF(I51="Arquitecto",Recursos!E$12,(IF(I51="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>31.977576754385964</v>
       </c>
-      <c r="K51" s="119">
+      <c r="K51" s="117">
         <f>F51*J51*G51</f>
         <v>0</v>
       </c>
@@ -6572,18 +6576,18 @@
       <c r="B52" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="114" t="s">
+      <c r="C52" s="112" t="s">
         <v>126</v>
       </c>
-      <c r="D52" s="115"/>
+      <c r="D52" s="113"/>
       <c r="E52" s="68"/>
-      <c r="F52" s="117">
-        <v>0</v>
-      </c>
-      <c r="G52" s="118">
+      <c r="F52" s="115">
+        <v>0</v>
+      </c>
+      <c r="G52" s="116">
         <v>1</v>
       </c>
-      <c r="H52" s="123" t="e">
+      <c r="H52" s="121" t="e">
         <f>(F52/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6594,7 +6598,7 @@
         <f>IF(I52="Líder de proyecto",Recursos!E$5,(IF(I52="Analista",Recursos!E$6,(IF(I52="Diseñador",Recursos!#REF!,(IF(I52="Tester",Recursos!E$7,(IF(I52="Desarrollador",Recursos!E$8,(IF(I52="Arquitecto",Recursos!E$12,(IF(I52="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>31.977576754385964</v>
       </c>
-      <c r="K52" s="119">
+      <c r="K52" s="117">
         <f>F52*J52*G52</f>
         <v>0</v>
       </c>
@@ -6603,18 +6607,18 @@
       <c r="B53" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="114" t="s">
+      <c r="C53" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="115"/>
+      <c r="D53" s="113"/>
       <c r="E53" s="68"/>
-      <c r="F53" s="117">
-        <v>0</v>
-      </c>
-      <c r="G53" s="118">
+      <c r="F53" s="115">
+        <v>0</v>
+      </c>
+      <c r="G53" s="116">
         <v>1</v>
       </c>
-      <c r="H53" s="123" t="e">
+      <c r="H53" s="121" t="e">
         <f>(F53/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6625,7 +6629,7 @@
         <f>IF(I53="Líder de proyecto",Recursos!E$5,(IF(I53="Analista",Recursos!E$6,(IF(I53="Diseñador",Recursos!#REF!,(IF(I53="Tester",Recursos!E$7,(IF(I53="Desarrollador",Recursos!E$8,(IF(I53="Arquitecto",Recursos!E$12,(IF(I53="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K53" s="119">
+      <c r="K53" s="117">
         <f>F53*J53*G53</f>
         <v>0</v>
       </c>
@@ -6634,18 +6638,18 @@
       <c r="B54" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="116" t="s">
+      <c r="C54" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="115"/>
+      <c r="D54" s="113"/>
       <c r="E54" s="68"/>
-      <c r="F54" s="117">
-        <v>0</v>
-      </c>
-      <c r="G54" s="120">
+      <c r="F54" s="115">
+        <v>0</v>
+      </c>
+      <c r="G54" s="118">
         <v>1</v>
       </c>
-      <c r="H54" s="123" t="e">
+      <c r="H54" s="121" t="e">
         <f>(F54/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6656,7 +6660,7 @@
         <f>IF(I54="Líder de proyecto",Recursos!E$5,(IF(I54="Analista",Recursos!E$6,(IF(I54="Diseñador",Recursos!#REF!,(IF(I54="Tester",Recursos!E$7,(IF(I54="Desarrollador",Recursos!E$8,(IF(I54="Arquitecto",Recursos!E$12,(IF(I54="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K54" s="119">
+      <c r="K54" s="117">
         <f>F54*J54*G54</f>
         <v>0</v>
       </c>
@@ -6664,28 +6668,28 @@
     </row>
     <row r="55" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
-      <c r="B55" s="128">
+      <c r="B55" s="126">
         <v>6</v>
       </c>
-      <c r="C55" s="129" t="s">
+      <c r="C55" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="D55" s="130"/>
-      <c r="E55" s="131"/>
-      <c r="F55" s="132">
+      <c r="D55" s="128"/>
+      <c r="E55" s="129"/>
+      <c r="F55" s="130">
         <v>6</v>
       </c>
-      <c r="G55" s="133">
+      <c r="G55" s="131">
         <v>1</v>
       </c>
-      <c r="H55" s="134" t="s">
+      <c r="H55" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="I55" s="235" t="s">
+      <c r="I55" s="239" t="s">
         <v>153</v>
       </c>
-      <c r="J55" s="236"/>
-      <c r="K55" s="135">
+      <c r="J55" s="240"/>
+      <c r="K55" s="133">
         <v>0</v>
       </c>
     </row>
@@ -6699,24 +6703,24 @@
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="241" t="s">
+      <c r="I56" s="245" t="s">
         <v>117</v>
       </c>
-      <c r="J56" s="241"/>
+      <c r="J56" s="245"/>
       <c r="K56" s="74">
         <f>SUM(K50+K47+K30+K16+K9+K55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B57" s="127"/>
+      <c r="B57" s="125"/>
       <c r="C57" s="55"/>
       <c r="D57" s="17"/>
-      <c r="I57" s="153" t="s">
+      <c r="I57" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="J57" s="154"/>
-      <c r="K57" s="155">
+      <c r="J57" s="151"/>
+      <c r="K57" s="152">
         <f>(200*F7)-K56</f>
         <v>0</v>
       </c>
@@ -6724,47 +6728,47 @@
     <row r="58" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C58" s="55"/>
       <c r="D58" s="17"/>
-      <c r="I58" s="150" t="s">
+      <c r="I58" s="147" t="s">
         <v>145</v>
       </c>
-      <c r="J58" s="151"/>
-      <c r="K58" s="152" t="s">
+      <c r="J58" s="148"/>
+      <c r="K58" s="149" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C59" s="55"/>
       <c r="D59" s="17"/>
-      <c r="I59" s="150"/>
-      <c r="J59" s="151"/>
-      <c r="K59" s="152">
+      <c r="I59" s="147"/>
+      <c r="J59" s="148"/>
+      <c r="K59" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C60" s="55"/>
       <c r="D60" s="17"/>
-      <c r="I60" s="150"/>
-      <c r="J60" s="151"/>
-      <c r="K60" s="152">
+      <c r="I60" s="147"/>
+      <c r="J60" s="148"/>
+      <c r="K60" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C61" s="55"/>
       <c r="D61" s="17"/>
-      <c r="I61" s="150"/>
-      <c r="J61" s="151"/>
-      <c r="K61" s="152">
+      <c r="I61" s="147"/>
+      <c r="J61" s="148"/>
+      <c r="K61" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C62" s="55"/>
       <c r="D62" s="17"/>
-      <c r="I62" s="150"/>
-      <c r="J62" s="151"/>
-      <c r="K62" s="152">
+      <c r="I62" s="147"/>
+      <c r="J62" s="148"/>
+      <c r="K62" s="149">
         <v>0</v>
       </c>
     </row>
@@ -6783,9 +6787,9 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="237"/>
-      <c r="D64" s="237"/>
-      <c r="I64" s="53" t="s">
+      <c r="C64" s="241"/>
+      <c r="D64" s="241"/>
+      <c r="I64" s="256" t="s">
         <v>79</v>
       </c>
       <c r="J64" s="1" t="s">
@@ -6821,7 +6825,7 @@
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="124" t="s">
+      <c r="B95" s="122" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6845,23 +6849,20 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51:G55 G45:G46 G37 G26:G29 G10:G15 G19:G24 G32:G35 G48:G49 G39:G43">
-      <formula1>1</formula1>
-      <formula2>10</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51">
+      <formula1>"Líder de proyecto, Analista, Arquitecto, Tester, Desarrollador,Administrador de la configuración, Aseguramiento de la calidad"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I52:I54 I10:I15 I18:I24 I26:I29 I37 I45:I46 I48:I49 I32:I35 I39:I43">
       <formula1>"Líder de proyecto, Analista, Arquitecto, Tester, Desarrollador, Aseguramiento de la calidad"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51">
-      <formula1>"Líder de proyecto, Analista, Arquitecto, Tester, Desarrollador,Administrador de la configuración, Aseguramiento de la calidad"</formula1>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51:G55 G45:G46 G37 G26:G29 G10:G15 G19:G24 G32:G35 G48:G49 G39:G43">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="K36 K38 K44 K47 K50" formula="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -6889,21 +6890,21 @@
     </row>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="153" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="153" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="156" t="s">
+      <c r="D4" s="153" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="157" t="s">
+      <c r="E4" s="154" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="110" t="s">
         <v>87</v>
       </c>
       <c r="C5" s="75">
@@ -6919,7 +6920,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="110" t="s">
         <v>88</v>
       </c>
       <c r="C6" s="75">
@@ -6935,7 +6936,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="110" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="75">
@@ -6951,7 +6952,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="123" t="s">
         <v>173</v>
       </c>
       <c r="C8" s="75">
@@ -6967,7 +6968,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="123" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="75">
@@ -6983,7 +6984,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="110" t="s">
         <v>90</v>
       </c>
       <c r="C10" s="75">
@@ -6999,7 +7000,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="123" t="s">
         <v>175</v>
       </c>
       <c r="C11" s="75">
@@ -7015,24 +7016,24 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="113" t="s">
+      <c r="B12" s="111" t="s">
         <v>157</v>
       </c>
       <c r="C12" s="75">
         <v>11788.65</v>
       </c>
-      <c r="D12" s="110">
+      <c r="D12" s="108">
         <f t="shared" si="1"/>
         <v>48.473067434210527</v>
       </c>
-      <c r="E12" s="111">
+      <c r="E12" s="109">
         <f t="shared" si="0"/>
         <v>59.853275767543863</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="155" t="s">
         <v>94</v>
       </c>
       <c r="C15" s="66" t="s">
@@ -7106,13 +7107,13 @@
     </row>
     <row r="26" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="159" t="s">
+      <c r="B27" s="156" t="s">
         <v>101</v>
       </c>
       <c r="C27" s="64">
         <v>8</v>
       </c>
-      <c r="D27" s="159" t="s">
+      <c r="D27" s="156" t="s">
         <v>102</v>
       </c>
       <c r="E27" s="78">
@@ -7126,6 +7127,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -7209,19 +7223,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7238,18 +7239,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7263,9 +7255,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Corregir detalles en las formulas
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/2. Estimación y Planeación/Plantillas estimación/PTLL_Estimación_Esfuerzo.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/2. Estimación y Planeación/Plantillas estimación/PTLL_Estimación_Esfuerzo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\Procesos\Ciclo de vida IWM\2. Estimación y Planeación\Plantillas estimación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Ciclo de vida IWM\2. Estimación y Planeación\Plantillas estimación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="193">
   <si>
     <t>Nº</t>
   </si>
@@ -1588,7 +1588,7 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1812,13 +1812,7 @@
     <xf numFmtId="49" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2098,9 +2092,6 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2117,92 +2108,99 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="27" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2245,13 +2243,6 @@
     <xf numFmtId="0" fontId="34" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="27" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="27" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3107,28 +3098,28 @@
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="165" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="164"/>
-      <c r="B2" s="216" t="s">
+    <row r="2" spans="1:7" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="162"/>
+      <c r="B2" s="218" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="216"/>
-      <c r="D2" s="217" t="s">
+      <c r="C2" s="218"/>
+      <c r="D2" s="219" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-    </row>
-    <row r="4" spans="1:7" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="162"/>
-      <c r="B4" s="166" t="s">
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+    </row>
+    <row r="4" spans="1:7" s="161" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="160"/>
+      <c r="B4" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -3167,15 +3158,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="162"/>
-      <c r="B12" s="166" t="s">
+    <row r="12" spans="1:7" s="161" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="160"/>
+      <c r="B12" s="164" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="162"/>
-      <c r="D12" s="162"/>
-      <c r="E12" s="162"/>
-      <c r="F12" s="162"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="160"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
@@ -3309,15 +3300,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:256" s="163" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A31" s="162"/>
-      <c r="B31" s="166" t="s">
+    <row r="31" spans="1:256" s="161" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="160"/>
+      <c r="B31" s="164" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="162"/>
-      <c r="D31" s="162"/>
-      <c r="E31" s="162"/>
-      <c r="F31" s="162"/>
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
     </row>
     <row r="32" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
@@ -3938,634 +3929,646 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="179" customWidth="1"/>
-    <col min="2" max="2" width="15" style="179" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="179" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="179" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="179" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="179" customWidth="1"/>
-    <col min="7" max="7" width="46.140625" style="179" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="179" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="179"/>
+    <col min="1" max="1" width="5.28515625" style="177" customWidth="1"/>
+    <col min="2" max="2" width="15" style="177" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" style="177" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="177" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="177" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="177" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" style="177" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="177" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="177"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="176" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="218" t="s">
+      <c r="B3" s="238" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="218"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="238"/>
+      <c r="E3" s="238"/>
+      <c r="F3" s="238"/>
+      <c r="G3" s="238"/>
+      <c r="H3" s="238"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="226" t="s">
+      <c r="B4" s="239" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
-      <c r="E4" s="226"/>
-      <c r="F4" s="226"/>
-      <c r="G4" s="226"/>
-      <c r="H4" s="226"/>
+      <c r="C4" s="239"/>
+      <c r="D4" s="239"/>
+      <c r="E4" s="239"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="239"/>
+      <c r="H4" s="239"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="239"/>
+      <c r="H5" s="239"/>
     </row>
     <row r="8" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="221" t="s">
+      <c r="B8" s="233" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="222"/>
-      <c r="D8" s="222"/>
-      <c r="E8" s="222"/>
-      <c r="F8" s="222"/>
-      <c r="G8" s="222"/>
-      <c r="H8" s="223"/>
+      <c r="C8" s="234"/>
+      <c r="D8" s="234"/>
+      <c r="E8" s="234"/>
+      <c r="F8" s="234"/>
+      <c r="G8" s="234"/>
+      <c r="H8" s="235"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="180"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181" t="s">
+      <c r="B9" s="178"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="182">
+      <c r="H9" s="180">
         <f>0.6+(0.01*SUM(F11:F23))</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="181" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="184" t="s">
+      <c r="C10" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="185" t="s">
+      <c r="D10" s="183" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="185" t="s">
+      <c r="E10" s="183" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="183" t="s">
+      <c r="F10" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="224" t="s">
+      <c r="G10" s="236" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="225"/>
+      <c r="H10" s="237"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="184" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="187" t="s">
+      <c r="C11" s="185" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="172">
+      <c r="D11" s="170">
         <v>2</v>
       </c>
-      <c r="E11" s="188">
-        <v>0</v>
-      </c>
-      <c r="F11" s="175">
+      <c r="E11" s="186">
+        <v>0</v>
+      </c>
+      <c r="F11" s="173">
         <f t="shared" ref="F11:F23" si="0">E11*D11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="227"/>
-      <c r="H11" s="228"/>
-      <c r="K11" s="189"/>
+      <c r="G11" s="231"/>
+      <c r="H11" s="232"/>
+      <c r="K11" s="187"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="190" t="s">
+      <c r="B12" s="188" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="189" t="s">
+      <c r="C12" s="187" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="173">
+      <c r="D12" s="171">
         <v>2</v>
       </c>
-      <c r="E12" s="191">
-        <v>0</v>
-      </c>
-      <c r="F12" s="176">
+      <c r="E12" s="189">
+        <v>0</v>
+      </c>
+      <c r="F12" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="219"/>
-      <c r="H12" s="220"/>
+      <c r="G12" s="222"/>
+      <c r="H12" s="223"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="188" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="189" t="s">
+      <c r="C13" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="173">
+      <c r="D13" s="171">
         <v>1</v>
       </c>
-      <c r="E13" s="191">
-        <v>0</v>
-      </c>
-      <c r="F13" s="176">
+      <c r="E13" s="189">
+        <v>0</v>
+      </c>
+      <c r="F13" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="219"/>
-      <c r="H13" s="220"/>
+      <c r="G13" s="222"/>
+      <c r="H13" s="223"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="190" t="s">
+      <c r="B14" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="189" t="s">
+      <c r="C14" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="173">
+      <c r="D14" s="171">
         <v>1</v>
       </c>
-      <c r="E14" s="191">
-        <v>0</v>
-      </c>
-      <c r="F14" s="176">
+      <c r="E14" s="189">
+        <v>0</v>
+      </c>
+      <c r="F14" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="219"/>
-      <c r="H14" s="220"/>
+      <c r="G14" s="222"/>
+      <c r="H14" s="223"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="190" t="s">
+      <c r="B15" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="189" t="s">
+      <c r="C15" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="173">
+      <c r="D15" s="171">
         <v>1</v>
       </c>
-      <c r="E15" s="191">
-        <v>0</v>
-      </c>
-      <c r="F15" s="176">
+      <c r="E15" s="189">
+        <v>0</v>
+      </c>
+      <c r="F15" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="219"/>
-      <c r="H15" s="220"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="223"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="190" t="s">
+      <c r="B16" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="189" t="s">
+      <c r="C16" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="173">
+      <c r="D16" s="171">
         <v>0.5</v>
       </c>
-      <c r="E16" s="191">
-        <v>0</v>
-      </c>
-      <c r="F16" s="176">
+      <c r="E16" s="189">
+        <v>0</v>
+      </c>
+      <c r="F16" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="189"/>
-      <c r="H16" s="192"/>
+      <c r="G16" s="187"/>
+      <c r="H16" s="190"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="190" t="s">
+      <c r="B17" s="188" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="189" t="s">
+      <c r="C17" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="173">
+      <c r="D17" s="171">
         <v>0.5</v>
       </c>
-      <c r="E17" s="191">
-        <v>0</v>
-      </c>
-      <c r="F17" s="176">
+      <c r="E17" s="189">
+        <v>0</v>
+      </c>
+      <c r="F17" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="219"/>
-      <c r="H17" s="220"/>
+      <c r="G17" s="222"/>
+      <c r="H17" s="223"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="190" t="s">
+      <c r="B18" s="188" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="189" t="s">
+      <c r="C18" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="173">
+      <c r="D18" s="171">
         <v>2</v>
       </c>
-      <c r="E18" s="191">
-        <v>0</v>
-      </c>
-      <c r="F18" s="176">
+      <c r="E18" s="189">
+        <v>0</v>
+      </c>
+      <c r="F18" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="189"/>
-      <c r="H18" s="192"/>
+      <c r="G18" s="187"/>
+      <c r="H18" s="190"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="190" t="s">
+      <c r="B19" s="188" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="189" t="s">
+      <c r="C19" s="187" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="173">
+      <c r="D19" s="171">
         <v>1</v>
       </c>
-      <c r="E19" s="191">
-        <v>0</v>
-      </c>
-      <c r="F19" s="176">
+      <c r="E19" s="189">
+        <v>0</v>
+      </c>
+      <c r="F19" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="219"/>
-      <c r="H19" s="220"/>
+      <c r="G19" s="222"/>
+      <c r="H19" s="223"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="190" t="s">
+      <c r="B20" s="188" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="189" t="s">
+      <c r="C20" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="173">
+      <c r="D20" s="171">
         <v>1</v>
       </c>
-      <c r="E20" s="191">
-        <v>0</v>
-      </c>
-      <c r="F20" s="176">
+      <c r="E20" s="189">
+        <v>0</v>
+      </c>
+      <c r="F20" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="219"/>
-      <c r="H20" s="220"/>
+      <c r="G20" s="222"/>
+      <c r="H20" s="223"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="190" t="s">
+      <c r="B21" s="188" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="189" t="s">
+      <c r="C21" s="187" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="173">
+      <c r="D21" s="171">
         <v>1</v>
       </c>
-      <c r="E21" s="191">
-        <v>0</v>
-      </c>
-      <c r="F21" s="176">
+      <c r="E21" s="189">
+        <v>0</v>
+      </c>
+      <c r="F21" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="219"/>
-      <c r="H21" s="220"/>
+      <c r="G21" s="222"/>
+      <c r="H21" s="223"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="190" t="s">
+      <c r="B22" s="188" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="189" t="s">
+      <c r="C22" s="187" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="173">
+      <c r="D22" s="171">
         <v>1</v>
       </c>
-      <c r="E22" s="191">
-        <v>0</v>
-      </c>
-      <c r="F22" s="176">
+      <c r="E22" s="189">
+        <v>0</v>
+      </c>
+      <c r="F22" s="174">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="219"/>
-      <c r="H22" s="220"/>
+      <c r="G22" s="222"/>
+      <c r="H22" s="223"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="193" t="s">
+      <c r="B23" s="191" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="194" t="s">
+      <c r="C23" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="174">
+      <c r="D23" s="172">
         <v>1</v>
       </c>
-      <c r="E23" s="195">
-        <v>0</v>
-      </c>
-      <c r="F23" s="177">
+      <c r="E23" s="193">
+        <v>0</v>
+      </c>
+      <c r="F23" s="175">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="219"/>
-      <c r="H23" s="220"/>
+      <c r="G23" s="222"/>
+      <c r="H23" s="223"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="196"/>
-      <c r="C24" s="197"/>
-      <c r="D24" s="197"/>
-      <c r="E24" s="197" t="s">
+      <c r="B24" s="194"/>
+      <c r="C24" s="195"/>
+      <c r="D24" s="195"/>
+      <c r="E24" s="195" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="198">
+      <c r="F24" s="196">
         <f>SUM(F11:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="197"/>
-      <c r="H24" s="199"/>
+      <c r="G24" s="195"/>
+      <c r="H24" s="197"/>
     </row>
     <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="233" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="222"/>
-      <c r="D27" s="222"/>
-      <c r="E27" s="222"/>
-      <c r="F27" s="222"/>
-      <c r="G27" s="222"/>
-      <c r="H27" s="223"/>
+      <c r="C27" s="234"/>
+      <c r="D27" s="234"/>
+      <c r="E27" s="234"/>
+      <c r="F27" s="234"/>
+      <c r="G27" s="234"/>
+      <c r="H27" s="235"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B28" s="181"/>
-      <c r="C28" s="181"/>
-      <c r="D28" s="181"/>
-      <c r="E28" s="181"/>
-      <c r="F28" s="181"/>
-      <c r="G28" s="181" t="s">
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="179"/>
+      <c r="E28" s="179"/>
+      <c r="F28" s="179"/>
+      <c r="G28" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="181">
+      <c r="H28" s="179">
         <f>1.4+(-0.03*SUM(F30:F37))</f>
         <v>1.4</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="183" t="s">
+      <c r="B29" s="181" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="184" t="s">
+      <c r="C29" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="185" t="s">
+      <c r="D29" s="183" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="185" t="s">
+      <c r="E29" s="183" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="183" t="s">
+      <c r="F29" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="224" t="s">
+      <c r="G29" s="236" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="225"/>
+      <c r="H29" s="237"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="186" t="s">
+      <c r="B30" s="184" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="200" t="s">
+      <c r="C30" s="198" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="207">
+      <c r="D30" s="205">
         <v>1.5</v>
       </c>
-      <c r="E30" s="188">
-        <v>0</v>
-      </c>
-      <c r="F30" s="201">
+      <c r="E30" s="186">
+        <v>0</v>
+      </c>
+      <c r="F30" s="199">
         <f t="shared" ref="F30:F37" si="1">E30*D30</f>
         <v>0</v>
       </c>
-      <c r="G30" s="227"/>
-      <c r="H30" s="228"/>
+      <c r="G30" s="231"/>
+      <c r="H30" s="232"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="190" t="s">
+      <c r="B31" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="189" t="s">
+      <c r="C31" s="187" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="208">
+      <c r="D31" s="206">
         <v>0.5</v>
       </c>
-      <c r="E31" s="191">
-        <v>0</v>
-      </c>
-      <c r="F31" s="202">
+      <c r="E31" s="189">
+        <v>0</v>
+      </c>
+      <c r="F31" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G31" s="219"/>
-      <c r="H31" s="220"/>
+      <c r="G31" s="222"/>
+      <c r="H31" s="223"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="190" t="s">
+      <c r="B32" s="188" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="189" t="s">
+      <c r="C32" s="187" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="208">
+      <c r="D32" s="206">
         <v>1</v>
       </c>
-      <c r="E32" s="191">
-        <v>0</v>
-      </c>
-      <c r="F32" s="202">
+      <c r="E32" s="189">
+        <v>0</v>
+      </c>
+      <c r="F32" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="219"/>
-      <c r="H32" s="220"/>
+      <c r="G32" s="222"/>
+      <c r="H32" s="223"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="190" t="s">
+      <c r="B33" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="189" t="s">
+      <c r="C33" s="187" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="208">
+      <c r="D33" s="206">
         <v>0.5</v>
       </c>
-      <c r="E33" s="191">
-        <v>0</v>
-      </c>
-      <c r="F33" s="202">
+      <c r="E33" s="189">
+        <v>0</v>
+      </c>
+      <c r="F33" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G33" s="219"/>
-      <c r="H33" s="220"/>
+      <c r="G33" s="222"/>
+      <c r="H33" s="223"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="190" t="s">
+      <c r="B34" s="188" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="189" t="s">
+      <c r="C34" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="208">
+      <c r="D34" s="206">
         <v>1</v>
       </c>
-      <c r="E34" s="191">
-        <v>0</v>
-      </c>
-      <c r="F34" s="202">
+      <c r="E34" s="189">
+        <v>0</v>
+      </c>
+      <c r="F34" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G34" s="219"/>
-      <c r="H34" s="220"/>
+      <c r="G34" s="222"/>
+      <c r="H34" s="223"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="190" t="s">
+      <c r="B35" s="188" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="189" t="s">
+      <c r="C35" s="187" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="208">
+      <c r="D35" s="206">
         <v>2</v>
       </c>
-      <c r="E35" s="191">
-        <v>0</v>
-      </c>
-      <c r="F35" s="202">
+      <c r="E35" s="189">
+        <v>0</v>
+      </c>
+      <c r="F35" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G35" s="189"/>
-      <c r="H35" s="192"/>
+      <c r="G35" s="187"/>
+      <c r="H35" s="190"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="190" t="s">
+      <c r="B36" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="189" t="s">
+      <c r="C36" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="208">
+      <c r="D36" s="206">
         <v>-1</v>
       </c>
-      <c r="E36" s="191">
-        <v>0</v>
-      </c>
-      <c r="F36" s="202">
+      <c r="E36" s="189">
+        <v>0</v>
+      </c>
+      <c r="F36" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36" s="219"/>
-      <c r="H36" s="220"/>
+      <c r="G36" s="222"/>
+      <c r="H36" s="223"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="190" t="s">
+      <c r="B37" s="188" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="189" t="s">
+      <c r="C37" s="187" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="208">
+      <c r="D37" s="206">
         <v>2</v>
       </c>
-      <c r="E37" s="191">
-        <v>0</v>
-      </c>
-      <c r="F37" s="202">
+      <c r="E37" s="189">
+        <v>0</v>
+      </c>
+      <c r="F37" s="200">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G37" s="189"/>
-      <c r="H37" s="192"/>
+      <c r="G37" s="187"/>
+      <c r="H37" s="190"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="196"/>
-      <c r="C38" s="203"/>
-      <c r="D38" s="197"/>
-      <c r="E38" s="203" t="s">
+      <c r="B38" s="194"/>
+      <c r="C38" s="201"/>
+      <c r="D38" s="195"/>
+      <c r="E38" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="198">
+      <c r="F38" s="196">
         <f>SUM(F30:F37)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="197"/>
-      <c r="H38" s="199"/>
+      <c r="G38" s="195"/>
+      <c r="H38" s="197"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="231" t="s">
+      <c r="B40" s="224" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="232"/>
-      <c r="F40" s="235" t="s">
+      <c r="C40" s="225"/>
+      <c r="F40" s="228" t="s">
         <v>66</v>
       </c>
-      <c r="G40" s="236"/>
-      <c r="H40" s="236"/>
+      <c r="G40" s="229"/>
+      <c r="H40" s="229"/>
     </row>
     <row r="41" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="233" t="s">
+      <c r="B41" s="226" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="234"/>
-      <c r="F41" s="233" t="s">
+      <c r="C41" s="227"/>
+      <c r="F41" s="226" t="s">
         <v>136</v>
       </c>
-      <c r="G41" s="237"/>
-      <c r="H41" s="237"/>
+      <c r="G41" s="230"/>
+      <c r="H41" s="230"/>
     </row>
     <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="204" t="s">
+      <c r="B42" s="202" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="205" t="s">
+      <c r="C42" s="203" t="s">
         <v>172</v>
       </c>
-      <c r="F42" s="206" t="s">
+      <c r="F42" s="204" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="229">
-        <v>0</v>
-      </c>
-      <c r="H42" s="230"/>
+      <c r="G42" s="220">
+        <v>0</v>
+      </c>
+      <c r="H42" s="221"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B4:H5"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="B40:C40"/>
@@ -4582,18 +4585,6 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B4:H5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -4630,45 +4621,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="240" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
+      <c r="C2" s="240"/>
+      <c r="D2" s="240"/>
+      <c r="E2" s="240"/>
+      <c r="F2" s="240"/>
+      <c r="G2" s="240"/>
     </row>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159" t="s">
+      <c r="B3" s="155"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="160">
+      <c r="G3" s="158">
         <f>SUM(G5:G29)*'Factor de complejidad Téc y Amb'!H9*'Factor de complejidad Téc y Amb'!H28</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="157" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="161" t="s">
+      <c r="B4" s="155" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="157" t="s">
+      <c r="D4" s="155" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="157" t="s">
+      <c r="E4" s="155" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="157" t="s">
+      <c r="F4" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="157" t="s">
+      <c r="G4" s="155" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4910,7 +4901,7 @@
       <c r="B18" s="2">
         <v>14</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="117" t="s">
         <v>79</v>
       </c>
       <c r="D18" s="11"/>
@@ -4928,7 +4919,7 @@
       <c r="B19" s="2">
         <v>15</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="117" t="s">
         <v>79</v>
       </c>
       <c r="D19" s="11"/>
@@ -4946,7 +4937,7 @@
       <c r="B20" s="2">
         <v>16</v>
       </c>
-      <c r="C20" s="119" t="s">
+      <c r="C20" s="117" t="s">
         <v>79</v>
       </c>
       <c r="D20" s="11"/>
@@ -5153,8 +5144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5280,25 +5271,25 @@
       <c r="P5" s="16"/>
     </row>
     <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="244" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="243"/>
-      <c r="J6" s="243"/>
-      <c r="K6" s="244"/>
+      <c r="C6" s="245"/>
+      <c r="D6" s="245"/>
+      <c r="E6" s="245"/>
+      <c r="F6" s="245"/>
+      <c r="G6" s="245"/>
+      <c r="H6" s="245"/>
+      <c r="I6" s="245"/>
+      <c r="J6" s="245"/>
+      <c r="K6" s="246"/>
     </row>
     <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="43"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
-      <c r="F7" s="120">
+      <c r="F7" s="118">
         <f>SUM(F9+F16+F30+F47+F50)</f>
         <v>0</v>
       </c>
@@ -5306,7 +5297,7 @@
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
-      <c r="K7" s="104"/>
+      <c r="K7" s="102"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
@@ -5336,40 +5327,40 @@
       <c r="J8" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="105" t="s">
+      <c r="K8" s="103" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="134">
+      <c r="B9" s="132">
         <v>1</v>
       </c>
-      <c r="C9" s="135" t="s">
+      <c r="C9" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="136"/>
-      <c r="E9" s="141" t="e">
+      <c r="D9" s="134"/>
+      <c r="E9" s="139" t="e">
         <f>(F9/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F9" s="144">
+      <c r="F9" s="142">
         <f>SUM(F10:F15)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="139"/>
-      <c r="H9" s="146"/>
-      <c r="I9" s="239" t="s">
+      <c r="G9" s="137"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="241" t="s">
         <v>118</v>
       </c>
-      <c r="J9" s="240"/>
-      <c r="K9" s="252">
-        <f>SUM(K10:K14)</f>
+      <c r="J9" s="242"/>
+      <c r="K9" s="213">
+        <f>SUM(K10:K15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
-      <c r="C10" s="167" t="s">
+      <c r="C10" s="165" t="s">
         <v>109</v>
       </c>
       <c r="D10" s="47"/>
@@ -5391,14 +5382,14 @@
         <f>IF(I10="Líder de proyecto",Recursos!E$5,(IF(I10="Analista",Recursos!E$6,(IF(I10="Diseñador",Recursos!#REF!,(IF(I10="Tester",Recursos!E$7,(IF(I10="Desarrollador",Recursos!E$8,(IF(I10="Arquitecto",Recursos!E$12,(IF(I10="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K10" s="106">
+      <c r="K10" s="104">
         <f t="shared" ref="K10:K15" si="0">F10*J10*G10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
-      <c r="C11" s="167" t="s">
+      <c r="C11" s="165" t="s">
         <v>110</v>
       </c>
       <c r="D11" s="47"/>
@@ -5420,14 +5411,14 @@
         <f>IF(I11="Líder de proyecto",Recursos!E$5,(IF(I11="Analista",Recursos!E$6,(IF(I11="Diseñador",Recursos!#REF!,(IF(I11="Tester",Recursos!E$7,(IF(I11="Desarrollador",Recursos!E$8,(IF(I11="Arquitecto",Recursos!E$12,(IF(I11="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K11" s="106">
+      <c r="K11" s="104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
-      <c r="C12" s="167" t="s">
+      <c r="C12" s="165" t="s">
         <v>171</v>
       </c>
       <c r="D12" s="47"/>
@@ -5449,14 +5440,14 @@
         <f>IF(I12="Líder de proyecto",Recursos!E$5,(IF(I12="Analista",Recursos!E$6,(IF(I12="Diseñador",Recursos!#REF!,(IF(I12="Tester",Recursos!E$7,(IF(I12="Desarrollador",Recursos!E$8,(IF(I12="Arquitecto",Recursos!E$12,(IF(I12="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K12" s="106">
+      <c r="K12" s="104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
-      <c r="C13" s="167" t="s">
+      <c r="C13" s="165" t="s">
         <v>113</v>
       </c>
       <c r="D13" s="47"/>
@@ -5478,14 +5469,14 @@
         <f>IF(I13="Líder de proyecto",Recursos!E$5,(IF(I13="Analista",Recursos!E$6,(IF(I13="Diseñador",Recursos!#REF!,(IF(I13="Tester",Recursos!E$7,(IF(I13="Desarrollador",Recursos!E$8,(IF(I13="Arquitecto",Recursos!E$12,(IF(I13="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K13" s="106">
+      <c r="K13" s="104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="47"/>
-      <c r="C14" s="167" t="s">
+      <c r="C14" s="165" t="s">
         <v>176</v>
       </c>
       <c r="D14" s="47"/>
@@ -5507,25 +5498,28 @@
         <f>IF(I14="Líder de proyecto",Recursos!E$5,(IF(I14="Analista",Recursos!E$6,(IF(I14="Diseñador",Recursos!#REF!,(IF(I14="Tester",Recursos!E$7,(IF(I14="Desarrollador",Recursos!E$8,(IF(I14="Arquitecto",Recursos!E$12,(IF(I14="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K14" s="106">
+      <c r="K14" s="104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
-      <c r="C15" s="167" t="s">
+      <c r="C15" s="165" t="s">
         <v>111</v>
       </c>
       <c r="D15" s="47"/>
-      <c r="E15" s="168"/>
+      <c r="E15" s="166"/>
       <c r="F15" s="51">
         <v>0</v>
       </c>
       <c r="G15" s="52">
         <v>1</v>
       </c>
-      <c r="H15" s="88"/>
+      <c r="H15" s="88" t="e">
+        <f>(F15/F9)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I15" s="81" t="s">
         <v>88</v>
       </c>
@@ -5533,36 +5527,36 @@
         <f>IF(I15="Líder de proyecto",Recursos!E$5,(IF(I15="Analista",Recursos!E$6,(IF(I15="Diseñador",Recursos!#REF!,(IF(I15="Tester",Recursos!E$7,(IF(I15="Desarrollador",Recursos!E$8,(IF(I15="Arquitecto",Recursos!E$12,(IF(I15="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K15" s="106">
+      <c r="K15" s="104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="134">
+      <c r="B16" s="132">
         <v>2</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C16" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="136"/>
-      <c r="E16" s="141" t="e">
+      <c r="D16" s="134"/>
+      <c r="E16" s="139" t="e">
         <f>(F16/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F16" s="144">
+      <c r="F16" s="142">
         <f>F17+F25</f>
         <v>0</v>
       </c>
-      <c r="G16" s="139"/>
-      <c r="H16" s="146"/>
-      <c r="I16" s="246" t="s">
+      <c r="G16" s="137"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="248" t="s">
         <v>119</v>
       </c>
-      <c r="J16" s="247" t="s">
+      <c r="J16" s="249" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="252">
+      <c r="K16" s="213">
         <f>SUM(K17+K25)</f>
         <v>0</v>
       </c>
@@ -5574,26 +5568,26 @@
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="68"/>
-      <c r="F17" s="211">
+      <c r="F17" s="208">
         <f>SUM(F18:F24)</f>
         <v>0</v>
       </c>
       <c r="G17" s="71"/>
       <c r="H17" s="72"/>
-      <c r="I17" s="248" t="s">
+      <c r="I17" s="250" t="s">
         <v>120</v>
       </c>
-      <c r="J17" s="249" t="s">
+      <c r="J17" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="253">
-        <f>SUM(K18:K25)</f>
+      <c r="K17" s="214">
+        <f>SUM(K18:K24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
-      <c r="C18" s="167" t="s">
+      <c r="C18" s="165" t="s">
         <v>177</v>
       </c>
       <c r="D18" s="47"/>
@@ -5615,14 +5609,14 @@
         <f>IF(I18="Líder de proyecto",Recursos!E$5,(IF(I18="Analista",Recursos!E$6,(IF(I18="Diseñador",Recursos!#REF!,(IF(I18="Tester",Recursos!E$7,(IF(I18="Desarrollador",Recursos!E$8,(IF(I18="Arquitecto",Recursos!E$12,(IF(I18="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K18" s="106">
+      <c r="K18" s="104">
         <f>F18*J18*G18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="47"/>
-      <c r="C19" s="167" t="s">
+      <c r="C19" s="165" t="s">
         <v>160</v>
       </c>
       <c r="D19" s="47"/>
@@ -5644,14 +5638,14 @@
         <f>IF(I19="Líder de proyecto",Recursos!E$5,(IF(I19="Analista",Recursos!E$6,(IF(I19="Diseñador",Recursos!#REF!,(IF(I19="Tester",Recursos!E$7,(IF(I19="Desarrollador",Recursos!E$8,(IF(I19="Arquitecto",Recursos!E$12,(IF(I19="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K19" s="106">
+      <c r="K19" s="104">
         <f>F19*J19*G19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="47"/>
-      <c r="C20" s="167" t="s">
+      <c r="C20" s="165" t="s">
         <v>112</v>
       </c>
       <c r="D20" s="47"/>
@@ -5673,14 +5667,14 @@
         <f>IF(I20="Líder de proyecto",Recursos!E$5,(IF(I20="Analista",Recursos!E$6,(IF(I20="Diseñador",Recursos!#REF!,(IF(I20="Tester",Recursos!E$7,(IF(I20="Desarrollador",Recursos!E$8,(IF(I20="Arquitecto",Recursos!E$12,(IF(I20="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K20" s="106">
+      <c r="K20" s="104">
         <f t="shared" ref="K20:K22" si="1">F20*J20*G20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="47"/>
-      <c r="C21" s="167" t="s">
+      <c r="C21" s="165" t="s">
         <v>178</v>
       </c>
       <c r="D21" s="47"/>
@@ -5702,11 +5696,11 @@
         <f>IF(I21="Líder de proyecto",Recursos!E$5,(IF(I21="Analista",Recursos!E$6,(IF(I21="Diseñador",Recursos!#REF!,(IF(I21="Tester",Recursos!E$7,(IF(I21="Desarrollador",Recursos!E$8,(IF(I21="Arquitecto",Recursos!E$12,(IF(I21="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K21" s="106">
+      <c r="K21" s="104">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N21" s="124" t="s">
+      <c r="N21" s="122" t="s">
         <v>79</v>
       </c>
       <c r="O21" s="1" t="s">
@@ -5715,7 +5709,7 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="47"/>
-      <c r="C22" s="167" t="s">
+      <c r="C22" s="165" t="s">
         <v>164</v>
       </c>
       <c r="D22" s="47"/>
@@ -5737,17 +5731,17 @@
         <f>IF(I22="Líder de proyecto",Recursos!E$5,(IF(I22="Analista",Recursos!E$6,(IF(I22="Diseñador",Recursos!#REF!,(IF(I22="Tester",Recursos!E$7,(IF(I22="Desarrollador",Recursos!E$8,(IF(I22="Arquitecto",Recursos!E$12,(IF(I22="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K22" s="106">
+      <c r="K22" s="104">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N22" s="124" t="s">
+      <c r="N22" s="122" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="47"/>
-      <c r="C23" s="167" t="s">
+      <c r="C23" s="165" t="s">
         <v>179</v>
       </c>
       <c r="D23" s="47"/>
@@ -5769,14 +5763,14 @@
         <f>IF(I23="Líder de proyecto",Recursos!E$5,(IF(I23="Analista",Recursos!E$6,(IF(I23="Diseñador",Recursos!#REF!,(IF(I23="Tester",Recursos!E$7,(IF(I23="Desarrollador",Recursos!E$8,(IF(I23="Arquitecto",Recursos!E$12,(IF(I23="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K23" s="107">
+      <c r="K23" s="105">
         <f>F23*J23*G23</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="47"/>
-      <c r="C24" s="169" t="s">
+      <c r="C24" s="167" t="s">
         <v>180</v>
       </c>
       <c r="D24" s="47"/>
@@ -5798,7 +5792,7 @@
         <f>IF(I24="Líder de proyecto",Recursos!E$5,(IF(I24="Analista",Recursos!E$6,(IF(I24="Diseñador",Recursos!#REF!,(IF(I24="Tester",Recursos!E$7,(IF(I24="Desarrollador",Recursos!E$8,(IF(I24="Arquitecto",Recursos!E$12,(IF(I24="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K24" s="107">
+      <c r="K24" s="105">
         <f>F24*J24*G24</f>
         <v>0</v>
       </c>
@@ -5810,26 +5804,26 @@
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="68"/>
-      <c r="F25" s="254">
+      <c r="F25" s="215">
         <f>SUM(F26:F29)</f>
         <v>0</v>
       </c>
       <c r="G25" s="71"/>
       <c r="H25" s="72"/>
-      <c r="I25" s="248" t="s">
+      <c r="I25" s="250" t="s">
         <v>121</v>
       </c>
-      <c r="J25" s="249" t="s">
+      <c r="J25" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="253">
+      <c r="K25" s="214">
         <f>SUM(K27:K28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="170"/>
-      <c r="C26" s="167" t="s">
+      <c r="B26" s="168"/>
+      <c r="C26" s="165" t="s">
         <v>181</v>
       </c>
       <c r="E26" s="68"/>
@@ -5840,7 +5834,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="88" t="e">
-        <f>(F26/F15)</f>
+        <f>(F26/F16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I26" s="81" t="s">
@@ -5850,14 +5844,14 @@
         <f>IF(I26="Líder de proyecto",Recursos!E$5,(IF(I26="Analista",Recursos!E$6,(IF(I26="Diseñador",Recursos!#REF!,(IF(I26="Tester",Recursos!E$7,(IF(I26="Desarrollador",Recursos!E$8,(IF(I26="Arquitecto",Recursos!E$12,(IF(I26="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K26" s="106">
+      <c r="K26" s="104">
         <f t="shared" ref="K26:K29" si="2">F26*J26*G26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="47"/>
-      <c r="C27" s="167" t="s">
+      <c r="C27" s="165" t="s">
         <v>154</v>
       </c>
       <c r="D27" s="47"/>
@@ -5879,14 +5873,14 @@
         <f>IF(I27="Líder de proyecto",Recursos!E$5,(IF(I27="Analista",Recursos!E$6,(IF(I27="Diseñador",Recursos!#REF!,(IF(I27="Tester",Recursos!E$7,(IF(I27="Desarrollador",Recursos!E$8,(IF(I27="Arquitecto",Recursos!E$12,(IF(I27="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K27" s="106">
+      <c r="K27" s="104">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="47"/>
-      <c r="C28" s="167" t="s">
+      <c r="C28" s="165" t="s">
         <v>192</v>
       </c>
       <c r="D28" s="47"/>
@@ -5908,18 +5902,18 @@
         <f>IF(I28="Líder de proyecto",Recursos!E$5,(IF(I28="Analista",Recursos!E$6,(IF(I28="Diseñador",Recursos!#REF!,(IF(I28="Tester",Recursos!E$7,(IF(I28="Desarrollador",Recursos!E$8,(IF(I28="Arquitecto",Recursos!E$12,(IF(I28="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K28" s="106">
+      <c r="K28" s="104">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="47"/>
-      <c r="C29" s="167" t="s">
+      <c r="C29" s="165" t="s">
         <v>155</v>
       </c>
       <c r="D29" s="47"/>
-      <c r="E29" s="168"/>
+      <c r="E29" s="166"/>
       <c r="F29" s="51">
         <v>0</v>
       </c>
@@ -5927,7 +5921,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="88" t="e">
-        <f>(F29/F17)</f>
+        <f>(F29/F16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I29" s="81" t="s">
@@ -5937,36 +5931,36 @@
         <f>IF(I29="Líder de proyecto",Recursos!E$5,(IF(I29="Analista",Recursos!E$6,(IF(I29="Diseñador",Recursos!#REF!,(IF(I29="Tester",Recursos!E$7,(IF(I29="Desarrollador",Recursos!E$8,(IF(I29="Arquitecto",Recursos!E$12,(IF(I29="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K29" s="106">
+      <c r="K29" s="104">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="134">
+      <c r="B30" s="132">
         <v>3</v>
       </c>
-      <c r="C30" s="135" t="s">
+      <c r="C30" s="133" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="142"/>
-      <c r="E30" s="143" t="e">
-        <f>SUM(E31+E36+E38+E45)</f>
+      <c r="D30" s="140"/>
+      <c r="E30" s="141" t="e">
+        <f>F30/F7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F30" s="144">
+      <c r="F30" s="142">
         <f>F31+F36+F38+F45</f>
         <v>0</v>
       </c>
-      <c r="G30" s="139"/>
-      <c r="H30" s="145"/>
-      <c r="I30" s="239" t="s">
+      <c r="G30" s="137"/>
+      <c r="H30" s="143"/>
+      <c r="I30" s="241" t="s">
         <v>158</v>
       </c>
-      <c r="J30" s="240" t="s">
+      <c r="J30" s="242" t="s">
         <v>79</v>
       </c>
-      <c r="K30" s="252">
+      <c r="K30" s="213">
         <f>SUM(K38+K36+K44+K31)</f>
         <v>0</v>
       </c>
@@ -5979,30 +5973,27 @@
         <v>165</v>
       </c>
       <c r="D31" s="59"/>
-      <c r="E31" s="103" t="e">
-        <f>(F31/F7)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E31" s="68"/>
       <c r="F31" s="73">
         <f>SUM(F32:F35)</f>
         <v>0</v>
       </c>
       <c r="G31" s="69"/>
       <c r="H31" s="83"/>
-      <c r="I31" s="250" t="s">
+      <c r="I31" s="252" t="s">
         <v>169</v>
       </c>
-      <c r="J31" s="251" t="s">
+      <c r="J31" s="253" t="s">
         <v>79</v>
       </c>
-      <c r="K31" s="255">
-        <f>K32</f>
+      <c r="K31" s="216">
+        <f>SUM(K32:K35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="54"/>
-      <c r="C32" s="167" t="s">
+      <c r="C32" s="165" t="s">
         <v>182</v>
       </c>
       <c r="D32" s="49"/>
@@ -6024,7 +6015,7 @@
         <f>IF(I32="Líder de proyecto",Recursos!E$5,(IF(I32="Analista",Recursos!E$6,(IF(I32="Diseñador",Recursos!#REF!,(IF(I32="Tester",Recursos!E$7,(IF(I32="Desarrollador",Recursos!E$8,(IF(I32="Arquitecto",Recursos!E$12,(IF(I32="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K32" s="106">
+      <c r="K32" s="104">
         <f>F32*J32*G32</f>
         <v>0</v>
       </c>
@@ -6034,7 +6025,7 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="54"/>
-      <c r="C33" s="167" t="s">
+      <c r="C33" s="165" t="s">
         <v>183</v>
       </c>
       <c r="D33" s="49"/>
@@ -6056,14 +6047,14 @@
         <f>IF(I33="Líder de proyecto",Recursos!E$5,(IF(I33="Analista",Recursos!E$6,(IF(I33="Diseñador",Recursos!#REF!,(IF(I33="Tester",Recursos!E$7,(IF(I33="Desarrollador",Recursos!E$8,(IF(I33="Arquitecto",Recursos!E$12,(IF(I33="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K33" s="106">
+      <c r="K33" s="104">
         <f t="shared" ref="K33:K35" si="3">F33*J33*G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="54"/>
-      <c r="C34" s="167" t="s">
+      <c r="C34" s="165" t="s">
         <v>184</v>
       </c>
       <c r="D34" s="49"/>
@@ -6085,14 +6076,14 @@
         <f>IF(I34="Líder de proyecto",Recursos!E$5,(IF(I34="Analista",Recursos!E$6,(IF(I34="Diseñador",Recursos!#REF!,(IF(I34="Tester",Recursos!E$7,(IF(I34="Desarrollador",Recursos!E$8,(IF(I34="Arquitecto",Recursos!E$12,(IF(I34="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K34" s="106">
+      <c r="K34" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="54"/>
-      <c r="C35" s="167" t="s">
+      <c r="C35" s="165" t="s">
         <v>185</v>
       </c>
       <c r="D35" s="49"/>
@@ -6114,7 +6105,7 @@
         <f>IF(I35="Líder de proyecto",Recursos!E$5,(IF(I35="Analista",Recursos!E$6,(IF(I35="Diseñador",Recursos!#REF!,(IF(I35="Tester",Recursos!E$7,(IF(I35="Desarrollador",Recursos!E$8,(IF(I35="Arquitecto",Recursos!E$12,(IF(I35="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K35" s="106">
+      <c r="K35" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6127,23 +6118,20 @@
         <v>166</v>
       </c>
       <c r="D36" s="59"/>
-      <c r="E36" s="103" t="e">
-        <f>(F36/F7)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E36" s="68"/>
       <c r="F36" s="73">
         <f>F37</f>
         <v>0</v>
       </c>
       <c r="G36" s="69"/>
       <c r="H36" s="61"/>
-      <c r="I36" s="250" t="s">
+      <c r="I36" s="252" t="s">
         <v>122</v>
       </c>
-      <c r="J36" s="251" t="s">
+      <c r="J36" s="253" t="s">
         <v>79</v>
       </c>
-      <c r="K36" s="255">
+      <c r="K36" s="216">
         <f>SUM(K37:K37)</f>
         <v>0</v>
       </c>
@@ -6154,7 +6142,7 @@
         <v>188</v>
       </c>
       <c r="D37" s="49"/>
-      <c r="E37" s="101"/>
+      <c r="E37" s="68"/>
       <c r="F37" s="51">
         <v>0</v>
       </c>
@@ -6172,7 +6160,7 @@
         <f>IF(I37="Líder de proyecto",Recursos!E$5,(IF(I37="Analista",Recursos!E$6,(IF(I37="Diseñador",Recursos!#REF!,(IF(I37="Tester",Recursos!E$7,(IF(I37="Desarrollador",Recursos!E$8,(IF(I37="Arquitecto",Recursos!E$12,(IF(I37="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K37" s="107">
+      <c r="K37" s="105">
         <f>F37*J37*G37</f>
         <v>0</v>
       </c>
@@ -6188,30 +6176,27 @@
         <v>167</v>
       </c>
       <c r="D38" s="62"/>
-      <c r="E38" s="103" t="e">
-        <f>(F38/F7)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E38" s="68"/>
       <c r="F38" s="91">
         <f>SUM(F39:F43)</f>
         <v>0</v>
       </c>
       <c r="G38" s="69"/>
       <c r="H38" s="61"/>
-      <c r="I38" s="250" t="s">
+      <c r="I38" s="252" t="s">
         <v>123</v>
       </c>
-      <c r="J38" s="251" t="s">
+      <c r="J38" s="253" t="s">
         <v>79</v>
       </c>
-      <c r="K38" s="255">
-        <f>SUM(K39:K42)</f>
+      <c r="K38" s="216">
+        <f>SUM(K39:K43)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="54"/>
-      <c r="C39" s="167" t="s">
+      <c r="C39" s="165" t="s">
         <v>161</v>
       </c>
       <c r="D39" s="50"/>
@@ -6233,7 +6218,7 @@
         <f>IF(I39="Líder de proyecto",Recursos!E$5,(IF(I39="Analista",Recursos!E$6,(IF(I39="Diseñador",Recursos!#REF!,(IF(I39="Tester",Recursos!E$7,(IF(I39="Desarrollador",Recursos!E$8,(IF(I39="Arquitecto",Recursos!E$12,(IF(I39="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K39" s="106">
+      <c r="K39" s="104">
         <f>F39*J39*G39</f>
         <v>0</v>
       </c>
@@ -6243,7 +6228,7 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="54"/>
-      <c r="C40" s="167" t="s">
+      <c r="C40" s="165" t="s">
         <v>116</v>
       </c>
       <c r="D40" s="50"/>
@@ -6265,14 +6250,14 @@
         <f>IF(I40="Líder de proyecto",Recursos!E$5,(IF(I40="Analista",Recursos!E$6,(IF(I40="Diseñador",Recursos!#REF!,(IF(I40="Tester",Recursos!E$7,(IF(I40="Desarrollador",Recursos!E$8,(IF(I40="Arquitecto",Recursos!E$12,(IF(I40="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K40" s="106">
+      <c r="K40" s="104">
         <f>F40*J40*G40</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="54"/>
-      <c r="C41" s="167" t="s">
+      <c r="C41" s="165" t="s">
         <v>159</v>
       </c>
       <c r="D41" s="50"/>
@@ -6294,14 +6279,14 @@
         <f>IF(I41="Líder de proyecto",Recursos!E$5,(IF(I41="Analista",Recursos!E$6,(IF(I41="Diseñador",Recursos!#REF!,(IF(I41="Tester",Recursos!E$7,(IF(I41="Desarrollador",Recursos!E$8,(IF(I41="Arquitecto",Recursos!E$12,(IF(I41="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K41" s="106">
+      <c r="K41" s="104">
         <f>F41*J41*G41</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="54"/>
-      <c r="C42" s="167" t="s">
+      <c r="C42" s="165" t="s">
         <v>190</v>
       </c>
       <c r="D42" s="50"/>
@@ -6323,32 +6308,40 @@
         <f>IF(I42="Líder de proyecto",Recursos!E$5,(IF(I42="Analista",Recursos!E$6,(IF(I42="Diseñador",Recursos!#REF!,(IF(I42="Tester",Recursos!E$7,(IF(I42="Desarrollador",Recursos!E$8,(IF(I42="Arquitecto",Recursos!E$12,(IF(I42="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K42" s="106">
+      <c r="K42" s="104">
         <f>F42*J42*G42</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="214"/>
-      <c r="B43" s="212"/>
-      <c r="C43" s="167" t="s">
+      <c r="A43" s="211"/>
+      <c r="B43" s="209"/>
+      <c r="C43" s="165" t="s">
         <v>191</v>
       </c>
-      <c r="D43" s="213"/>
+      <c r="D43" s="210"/>
       <c r="E43" s="68"/>
-      <c r="F43" s="210">
-        <v>0</v>
-      </c>
-      <c r="G43" s="215">
+      <c r="F43" s="207">
+        <v>0</v>
+      </c>
+      <c r="G43" s="212">
         <v>1</v>
       </c>
       <c r="H43" s="88" t="e">
         <f>F43/F30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I43" s="81"/>
-      <c r="J43" s="82"/>
-      <c r="K43" s="106"/>
+      <c r="I43" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="J43" s="82">
+        <f>IF(I43="Líder de proyecto",Recursos!E$5,(IF(I43="Analista",Recursos!E$6,(IF(I43="Diseñador",Recursos!#REF!,(IF(I43="Tester",Recursos!E$7,(IF(I43="Desarrollador",Recursos!E$8,(IF(I43="Arquitecto",Recursos!E$12,(IF(I43="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>51.617173793859649</v>
+      </c>
+      <c r="K43" s="104">
+        <f>F43*J43*G43</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="54">
@@ -6358,23 +6351,20 @@
         <v>168</v>
       </c>
       <c r="D44" s="60"/>
-      <c r="E44" s="209" t="e">
-        <f>(F44/F7)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E44" s="68"/>
       <c r="F44" s="73">
         <f>SUM(F45:F46)</f>
         <v>0</v>
       </c>
       <c r="G44" s="69"/>
       <c r="H44" s="89"/>
-      <c r="I44" s="250" t="s">
+      <c r="I44" s="252" t="s">
         <v>124</v>
       </c>
-      <c r="J44" s="251" t="s">
+      <c r="J44" s="253" t="s">
         <v>79</v>
       </c>
-      <c r="K44" s="255">
+      <c r="K44" s="216">
         <f>SUM(K45:K46)</f>
         <v>0</v>
       </c>
@@ -6392,8 +6382,9 @@
       <c r="G45" s="56">
         <v>1</v>
       </c>
-      <c r="H45" s="88">
-        <v>0.5</v>
+      <c r="H45" s="88" t="e">
+        <f>F45/F30</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I45" s="81" t="s">
         <v>157</v>
@@ -6402,7 +6393,7 @@
         <f>IF(I45="Líder de proyecto",Recursos!E$5,(IF(I45="Analista",Recursos!E$6,(IF(I45="Diseñador",Recursos!#REF!,(IF(I45="Tester",Recursos!E$7,(IF(I45="Desarrollador",Recursos!E$8,(IF(I45="Arquitecto",Recursos!E$12,(IF(I45="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K45" s="106">
+      <c r="K45" s="104">
         <f>F45*J45*G45</f>
         <v>0</v>
       </c>
@@ -6420,8 +6411,9 @@
       <c r="G46" s="56">
         <v>1</v>
       </c>
-      <c r="H46" s="88">
-        <v>0.5</v>
+      <c r="H46" s="88" t="e">
+        <f>F46/F30</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I46" s="81" t="s">
         <v>88</v>
@@ -6430,37 +6422,37 @@
         <f>IF(I46="Líder de proyecto",Recursos!E$5,(IF(I46="Analista",Recursos!E$6,(IF(I46="Diseñador",Recursos!#REF!,(IF(I46="Tester",Recursos!E$7,(IF(I46="Desarrollador",Recursos!E$8,(IF(I46="Arquitecto",Recursos!E$12,(IF(I46="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>51.617173793859649</v>
       </c>
-      <c r="K46" s="106">
+      <c r="K46" s="104">
         <f>F46*J46*G46</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="134">
+      <c r="B47" s="132">
         <v>4</v>
       </c>
-      <c r="C47" s="135" t="s">
+      <c r="C47" s="133" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="136"/>
-      <c r="E47" s="141" t="e">
+      <c r="D47" s="134"/>
+      <c r="E47" s="139" t="e">
         <f>(F47/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F47" s="138">
+      <c r="F47" s="136">
         <f>F48+F49</f>
         <v>0</v>
       </c>
-      <c r="G47" s="139"/>
-      <c r="H47" s="140"/>
-      <c r="I47" s="239" t="s">
+      <c r="G47" s="137"/>
+      <c r="H47" s="138"/>
+      <c r="I47" s="241" t="s">
         <v>125</v>
       </c>
-      <c r="J47" s="240" t="s">
+      <c r="J47" s="242" t="s">
         <v>79</v>
       </c>
-      <c r="K47" s="252">
-        <f>SUM(K48:K48)</f>
+      <c r="K47" s="213">
+        <f>SUM(K48:K49)</f>
         <v>0</v>
       </c>
     </row>
@@ -6468,19 +6460,20 @@
       <c r="B48" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="167" t="s">
+      <c r="C48" s="165" t="s">
         <v>186</v>
       </c>
       <c r="D48" s="47"/>
-      <c r="E48" s="171"/>
+      <c r="E48" s="169"/>
       <c r="F48" s="51">
         <v>0</v>
       </c>
       <c r="G48" s="52">
         <v>1</v>
       </c>
-      <c r="H48" s="90">
-        <v>1</v>
+      <c r="H48" s="90" t="e">
+        <f>F48/F47</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I48" s="81" t="s">
         <v>87</v>
@@ -6489,74 +6482,83 @@
         <f>IF(I48="Líder de proyecto",Recursos!E$5,(IF(I48="Analista",Recursos!E$6,(IF(I48="Diseñador",Recursos!#REF!,(IF(I48="Tester",Recursos!E$7,(IF(I48="Desarrollador",Recursos!E$8,(IF(I48="Arquitecto",Recursos!E$12,(IF(I48="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K48" s="106">
+      <c r="K48" s="104">
         <f>F48*J48*G48</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="47"/>
-      <c r="C49" s="167" t="s">
+      <c r="C49" s="165" t="s">
         <v>187</v>
       </c>
       <c r="D49" s="47"/>
-      <c r="E49" s="171"/>
+      <c r="E49" s="169"/>
       <c r="F49" s="51">
         <v>0</v>
       </c>
       <c r="G49" s="52">
         <v>1</v>
       </c>
-      <c r="H49" s="90">
-        <v>1</v>
-      </c>
-      <c r="I49" s="81"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="106"/>
+      <c r="H49" s="90" t="e">
+        <f>F49/F47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="J49" s="82">
+        <f>IF(I49="Líder de proyecto",Recursos!E$5,(IF(I49="Analista",Recursos!E$6,(IF(I49="Diseñador",Recursos!#REF!,(IF(I49="Tester",Recursos!E$7,(IF(I49="Desarrollador",Recursos!E$8,(IF(I49="Arquitecto",Recursos!E$12,(IF(I49="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>59.853275767543863</v>
+      </c>
+      <c r="K49" s="104">
+        <f>F49*J49*G49</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="134">
+      <c r="B50" s="132">
         <v>5</v>
       </c>
-      <c r="C50" s="135" t="s">
+      <c r="C50" s="133" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="136"/>
-      <c r="E50" s="137" t="e">
+      <c r="D50" s="134"/>
+      <c r="E50" s="135" t="e">
         <f>(F50/F7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F50" s="138">
+      <c r="F50" s="136">
         <f>SUM(F51:F54)</f>
         <v>0</v>
       </c>
-      <c r="G50" s="139"/>
-      <c r="H50" s="140"/>
-      <c r="I50" s="239" t="s">
+      <c r="G50" s="137"/>
+      <c r="H50" s="138"/>
+      <c r="I50" s="241" t="s">
         <v>134</v>
       </c>
-      <c r="J50" s="240" t="s">
+      <c r="J50" s="242" t="s">
         <v>79</v>
       </c>
-      <c r="K50" s="252">
+      <c r="K50" s="213">
         <f>SUM(K51:K54)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="63"/>
-      <c r="C51" s="112" t="s">
+      <c r="C51" s="110" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="113"/>
+      <c r="D51" s="111"/>
       <c r="E51" s="68"/>
-      <c r="F51" s="115">
-        <v>0</v>
-      </c>
-      <c r="G51" s="116">
+      <c r="F51" s="113">
+        <v>0</v>
+      </c>
+      <c r="G51" s="114">
         <v>1</v>
       </c>
-      <c r="H51" s="121" t="e">
+      <c r="H51" s="119" t="e">
         <f>(F51/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6567,7 +6569,7 @@
         <f>IF(I51="Líder de proyecto",Recursos!E$5,(IF(I51="Analista",Recursos!E$6,(IF(I51="Administrador de la configuración",Recursos!E$11,(IF(I51="Tester",Recursos!E$7,(IF(I51="Desarrollador",Recursos!E$8,(IF(I51="Arquitecto",Recursos!E$12,(IF(I51="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>31.977576754385964</v>
       </c>
-      <c r="K51" s="117">
+      <c r="K51" s="115">
         <f>F51*J51*G51</f>
         <v>0</v>
       </c>
@@ -6576,18 +6578,18 @@
       <c r="B52" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="112" t="s">
+      <c r="C52" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="D52" s="113"/>
+      <c r="D52" s="111"/>
       <c r="E52" s="68"/>
-      <c r="F52" s="115">
-        <v>0</v>
-      </c>
-      <c r="G52" s="116">
+      <c r="F52" s="113">
+        <v>0</v>
+      </c>
+      <c r="G52" s="114">
         <v>1</v>
       </c>
-      <c r="H52" s="121" t="e">
+      <c r="H52" s="119" t="e">
         <f>(F52/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6598,7 +6600,7 @@
         <f>IF(I52="Líder de proyecto",Recursos!E$5,(IF(I52="Analista",Recursos!E$6,(IF(I52="Diseñador",Recursos!#REF!,(IF(I52="Tester",Recursos!E$7,(IF(I52="Desarrollador",Recursos!E$8,(IF(I52="Arquitecto",Recursos!E$12,(IF(I52="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>31.977576754385964</v>
       </c>
-      <c r="K52" s="117">
+      <c r="K52" s="115">
         <f>F52*J52*G52</f>
         <v>0</v>
       </c>
@@ -6607,18 +6609,18 @@
       <c r="B53" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="112" t="s">
+      <c r="C53" s="110" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="113"/>
+      <c r="D53" s="111"/>
       <c r="E53" s="68"/>
-      <c r="F53" s="115">
-        <v>0</v>
-      </c>
-      <c r="G53" s="116">
+      <c r="F53" s="113">
+        <v>0</v>
+      </c>
+      <c r="G53" s="114">
         <v>1</v>
       </c>
-      <c r="H53" s="121" t="e">
+      <c r="H53" s="119" t="e">
         <f>(F53/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6629,27 +6631,27 @@
         <f>IF(I53="Líder de proyecto",Recursos!E$5,(IF(I53="Analista",Recursos!E$6,(IF(I53="Diseñador",Recursos!#REF!,(IF(I53="Tester",Recursos!E$7,(IF(I53="Desarrollador",Recursos!E$8,(IF(I53="Arquitecto",Recursos!E$12,(IF(I53="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K53" s="117">
+      <c r="K53" s="115">
         <f>F53*J53*G53</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="102" t="s">
+      <c r="B54" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="114" t="s">
+      <c r="C54" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="113"/>
+      <c r="D54" s="111"/>
       <c r="E54" s="68"/>
-      <c r="F54" s="115">
-        <v>0</v>
-      </c>
-      <c r="G54" s="118">
+      <c r="F54" s="113">
+        <v>0</v>
+      </c>
+      <c r="G54" s="116">
         <v>1</v>
       </c>
-      <c r="H54" s="121" t="e">
+      <c r="H54" s="119" t="e">
         <f>(F54/F50)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6660,7 +6662,7 @@
         <f>IF(I54="Líder de proyecto",Recursos!E$5,(IF(I54="Analista",Recursos!E$6,(IF(I54="Diseñador",Recursos!#REF!,(IF(I54="Tester",Recursos!E$7,(IF(I54="Desarrollador",Recursos!E$8,(IF(I54="Arquitecto",Recursos!E$12,(IF(I54="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
         <v>59.853275767543863</v>
       </c>
-      <c r="K54" s="117">
+      <c r="K54" s="115">
         <f>F54*J54*G54</f>
         <v>0</v>
       </c>
@@ -6668,28 +6670,28 @@
     </row>
     <row r="55" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
-      <c r="B55" s="126">
+      <c r="B55" s="124">
         <v>6</v>
       </c>
-      <c r="C55" s="127" t="s">
+      <c r="C55" s="125" t="s">
         <v>152</v>
       </c>
-      <c r="D55" s="128"/>
-      <c r="E55" s="129"/>
-      <c r="F55" s="130">
+      <c r="D55" s="126"/>
+      <c r="E55" s="127"/>
+      <c r="F55" s="128">
         <v>6</v>
       </c>
-      <c r="G55" s="131">
+      <c r="G55" s="129">
         <v>1</v>
       </c>
-      <c r="H55" s="132" t="s">
+      <c r="H55" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="I55" s="239" t="s">
+      <c r="I55" s="241" t="s">
         <v>153</v>
       </c>
-      <c r="J55" s="240"/>
-      <c r="K55" s="133">
+      <c r="J55" s="242"/>
+      <c r="K55" s="131">
         <v>0</v>
       </c>
     </row>
@@ -6703,24 +6705,24 @@
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="245" t="s">
+      <c r="I56" s="247" t="s">
         <v>117</v>
       </c>
-      <c r="J56" s="245"/>
+      <c r="J56" s="247"/>
       <c r="K56" s="74">
         <f>SUM(K50+K47+K30+K16+K9+K55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B57" s="125"/>
+      <c r="B57" s="123"/>
       <c r="C57" s="55"/>
       <c r="D57" s="17"/>
-      <c r="I57" s="150" t="s">
+      <c r="I57" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="J57" s="151"/>
-      <c r="K57" s="152">
+      <c r="J57" s="149"/>
+      <c r="K57" s="150">
         <f>(200*F7)-K56</f>
         <v>0</v>
       </c>
@@ -6728,47 +6730,47 @@
     <row r="58" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C58" s="55"/>
       <c r="D58" s="17"/>
-      <c r="I58" s="147" t="s">
+      <c r="I58" s="145" t="s">
         <v>145</v>
       </c>
-      <c r="J58" s="148"/>
-      <c r="K58" s="149" t="s">
+      <c r="J58" s="146"/>
+      <c r="K58" s="147" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C59" s="55"/>
       <c r="D59" s="17"/>
-      <c r="I59" s="147"/>
-      <c r="J59" s="148"/>
-      <c r="K59" s="149">
+      <c r="I59" s="145"/>
+      <c r="J59" s="146"/>
+      <c r="K59" s="147">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C60" s="55"/>
       <c r="D60" s="17"/>
-      <c r="I60" s="147"/>
-      <c r="J60" s="148"/>
-      <c r="K60" s="149">
+      <c r="I60" s="145"/>
+      <c r="J60" s="146"/>
+      <c r="K60" s="147">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C61" s="55"/>
       <c r="D61" s="17"/>
-      <c r="I61" s="147"/>
-      <c r="J61" s="148"/>
-      <c r="K61" s="149">
+      <c r="I61" s="145"/>
+      <c r="J61" s="146"/>
+      <c r="K61" s="147">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="C62" s="55"/>
       <c r="D62" s="17"/>
-      <c r="I62" s="147"/>
-      <c r="J62" s="148"/>
-      <c r="K62" s="149">
+      <c r="I62" s="145"/>
+      <c r="J62" s="146"/>
+      <c r="K62" s="147">
         <v>0</v>
       </c>
     </row>
@@ -6787,9 +6789,9 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="241"/>
-      <c r="D64" s="241"/>
-      <c r="I64" s="256" t="s">
+      <c r="C64" s="243"/>
+      <c r="D64" s="243"/>
+      <c r="I64" s="217" t="s">
         <v>79</v>
       </c>
       <c r="J64" s="1" t="s">
@@ -6825,7 +6827,7 @@
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="122" t="s">
+      <c r="B95" s="120" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6890,21 +6892,21 @@
     </row>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="151" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="151" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="154" t="s">
+      <c r="E4" s="152" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="108" t="s">
         <v>87</v>
       </c>
       <c r="C5" s="75">
@@ -6920,7 +6922,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="108" t="s">
         <v>88</v>
       </c>
       <c r="C6" s="75">
@@ -6936,7 +6938,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="108" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="75">
@@ -6952,7 +6954,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="121" t="s">
         <v>173</v>
       </c>
       <c r="C8" s="75">
@@ -6968,7 +6970,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="121" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="75">
@@ -6984,7 +6986,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="110" t="s">
+      <c r="B10" s="108" t="s">
         <v>90</v>
       </c>
       <c r="C10" s="75">
@@ -7000,7 +7002,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="121" t="s">
         <v>175</v>
       </c>
       <c r="C11" s="75">
@@ -7016,24 +7018,24 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="109" t="s">
         <v>157</v>
       </c>
       <c r="C12" s="75">
         <v>11788.65</v>
       </c>
-      <c r="D12" s="108">
+      <c r="D12" s="106">
         <f t="shared" si="1"/>
         <v>48.473067434210527</v>
       </c>
-      <c r="E12" s="109">
+      <c r="E12" s="107">
         <f t="shared" si="0"/>
         <v>59.853275767543863</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="153" t="s">
         <v>94</v>
       </c>
       <c r="C15" s="66" t="s">
@@ -7107,13 +7109,13 @@
     </row>
     <row r="26" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="154" t="s">
         <v>101</v>
       </c>
       <c r="C27" s="64">
         <v>8</v>
       </c>
-      <c r="D27" s="156" t="s">
+      <c r="D27" s="154" t="s">
         <v>102</v>
       </c>
       <c r="E27" s="78">
@@ -7127,19 +7129,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
+    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -7223,38 +7227,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
-    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7271,18 +7273,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>